<commit_message>
update code and result
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="42">
   <si>
     <t>图</t>
     <rPh sb="0" eb="1">
@@ -205,11 +205,22 @@
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>IMP LCTES</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IMP BaseLine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0.000_ "/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -247,11 +258,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -532,7 +545,7 @@
   <dimension ref="A1:T103"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="R99" sqref="R99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -571,10 +584,10 @@
         <v>31</v>
       </c>
       <c r="B2">
+        <v>10000</v>
+      </c>
+      <c r="C2">
         <v>100000</v>
-      </c>
-      <c r="C2">
-        <v>1000000</v>
       </c>
       <c r="D2">
         <v>20480</v>
@@ -606,12 +619,12 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -695,7 +708,34 @@
         <v>177</v>
       </c>
       <c r="F5">
-        <v>28945000</v>
+        <v>29120000</v>
+      </c>
+      <c r="G5">
+        <v>15995000</v>
+      </c>
+      <c r="H5">
+        <v>10080000</v>
+      </c>
+      <c r="I5">
+        <v>49150800</v>
+      </c>
+      <c r="J5">
+        <v>47058000</v>
+      </c>
+      <c r="K5">
+        <v>47023632</v>
+      </c>
+      <c r="O5" s="2">
+        <f>(I5-F5)/I5</f>
+        <v>0.40753761891973272</v>
+      </c>
+      <c r="P5" s="2">
+        <f t="shared" ref="P5:Q18" si="0">(J5-G5)/J5</f>
+        <v>0.66010030175528067</v>
+      </c>
+      <c r="Q5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.78563969707826908</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -715,7 +755,34 @@
         <v>154</v>
       </c>
       <c r="F6">
-        <v>23940000</v>
+        <v>23730000</v>
+      </c>
+      <c r="G6">
+        <v>13230000</v>
+      </c>
+      <c r="H6">
+        <v>7980000</v>
+      </c>
+      <c r="I6">
+        <v>51108000</v>
+      </c>
+      <c r="J6">
+        <v>51102600</v>
+      </c>
+      <c r="K6">
+        <v>51442076</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" ref="O6:O18" si="1">(I6-F6)/I6</f>
+        <v>0.53568912890349851</v>
+      </c>
+      <c r="P6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.74110906294395984</v>
+      </c>
+      <c r="Q6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.84487406767953921</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -735,7 +802,34 @@
         <v>118</v>
       </c>
       <c r="F7">
-        <v>25728300</v>
+        <v>25517700</v>
+      </c>
+      <c r="G7">
+        <v>13889850</v>
+      </c>
+      <c r="H7">
+        <v>8247627</v>
+      </c>
+      <c r="I7">
+        <v>79027200</v>
+      </c>
+      <c r="J7">
+        <v>78986880</v>
+      </c>
+      <c r="K7">
+        <v>78974112</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="1"/>
+        <v>0.67710231413994171</v>
+      </c>
+      <c r="P7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.82414990945331679</v>
+      </c>
+      <c r="Q7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.89556543541762146</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -752,10 +846,37 @@
         <v>1471</v>
       </c>
       <c r="E8">
-        <v>1471</v>
+        <v>440</v>
       </c>
       <c r="F8">
-        <v>30080070</v>
+        <v>30150930</v>
+      </c>
+      <c r="G8">
+        <v>16864680</v>
+      </c>
+      <c r="H8">
+        <v>10221555</v>
+      </c>
+      <c r="I8">
+        <v>190618500</v>
+      </c>
+      <c r="J8">
+        <v>190416500</v>
+      </c>
+      <c r="K8">
+        <v>190325500</v>
+      </c>
+      <c r="O8" s="2">
+        <f t="shared" si="1"/>
+        <v>0.84182579340410291</v>
+      </c>
+      <c r="P8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.91143267521459537</v>
+      </c>
+      <c r="Q8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.94629434836635129</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
@@ -775,7 +896,34 @@
         <v>117</v>
       </c>
       <c r="F9">
-        <v>755014</v>
+        <v>754196</v>
+      </c>
+      <c r="G9">
+        <v>403274</v>
+      </c>
+      <c r="H9">
+        <v>233130</v>
+      </c>
+      <c r="I9">
+        <v>14247000</v>
+      </c>
+      <c r="J9">
+        <v>14229000</v>
+      </c>
+      <c r="K9">
+        <v>7122484</v>
+      </c>
+      <c r="O9" s="2">
+        <f t="shared" si="1"/>
+        <v>0.94706282024285815</v>
+      </c>
+      <c r="P9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.97165830346475512</v>
+      </c>
+      <c r="Q9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.96726844174026927</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -795,7 +943,34 @@
         <v>235</v>
       </c>
       <c r="F10">
-        <v>52216164</v>
+        <v>52413504</v>
+      </c>
+      <c r="G10">
+        <v>28203674</v>
+      </c>
+      <c r="H10">
+        <v>16905000</v>
+      </c>
+      <c r="I10">
+        <v>96700500</v>
+      </c>
+      <c r="J10">
+        <v>92270664</v>
+      </c>
+      <c r="K10">
+        <v>92066512</v>
+      </c>
+      <c r="O10" s="2">
+        <f t="shared" si="1"/>
+        <v>0.45798104456543659</v>
+      </c>
+      <c r="P10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.69433758491214503</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.81638274729035021</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
@@ -817,6 +992,33 @@
       <c r="F11">
         <v>26821144</v>
       </c>
+      <c r="G11">
+        <v>14601944</v>
+      </c>
+      <c r="H11">
+        <v>8492344</v>
+      </c>
+      <c r="I11">
+        <v>66295704</v>
+      </c>
+      <c r="J11">
+        <v>33703560</v>
+      </c>
+      <c r="K11">
+        <v>22845232</v>
+      </c>
+      <c r="O11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.59543164365522083</v>
+      </c>
+      <c r="P11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.56675366044417863</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.628266239537423</v>
+      </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -834,6 +1036,36 @@
       <c r="E12">
         <v>189</v>
       </c>
+      <c r="F12">
+        <v>29295000</v>
+      </c>
+      <c r="G12">
+        <v>16170000</v>
+      </c>
+      <c r="H12">
+        <v>10255000</v>
+      </c>
+      <c r="I12">
+        <v>89291792</v>
+      </c>
+      <c r="J12">
+        <v>89263216</v>
+      </c>
+      <c r="K12">
+        <v>89249232</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.67191833265032919</v>
+      </c>
+      <c r="P12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.81885035376722259</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.88509705047097775</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -848,6 +1080,39 @@
       <c r="D13">
         <v>747</v>
       </c>
+      <c r="E13">
+        <v>190</v>
+      </c>
+      <c r="F13">
+        <v>27745458</v>
+      </c>
+      <c r="G13">
+        <v>15715000</v>
+      </c>
+      <c r="H13">
+        <v>9555000</v>
+      </c>
+      <c r="I13">
+        <v>73170976</v>
+      </c>
+      <c r="J13">
+        <v>72663616</v>
+      </c>
+      <c r="K13">
+        <v>73132976</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="1"/>
+        <v>0.62081333997786226</v>
+      </c>
+      <c r="P13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.78372945271537275</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.86934758405018275</v>
+      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -862,6 +1127,39 @@
       <c r="D14">
         <v>855</v>
       </c>
+      <c r="E14">
+        <v>200</v>
+      </c>
+      <c r="F14">
+        <v>33600000</v>
+      </c>
+      <c r="G14">
+        <v>18585000</v>
+      </c>
+      <c r="H14">
+        <v>11095000</v>
+      </c>
+      <c r="I14">
+        <v>93739312</v>
+      </c>
+      <c r="J14">
+        <v>93094520</v>
+      </c>
+      <c r="K14">
+        <v>93697664</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.64155913582979995</v>
+      </c>
+      <c r="P14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.80036418899845019</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.8815872293251622</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -876,6 +1174,39 @@
       <c r="D15">
         <v>1017</v>
       </c>
+      <c r="E15">
+        <v>215</v>
+      </c>
+      <c r="F15">
+        <v>34700864</v>
+      </c>
+      <c r="G15">
+        <v>20020000</v>
+      </c>
+      <c r="H15">
+        <v>11935000</v>
+      </c>
+      <c r="I15">
+        <v>97975856</v>
+      </c>
+      <c r="J15">
+        <v>97298964</v>
+      </c>
+      <c r="K15">
+        <v>97927824</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.64582229319843865</v>
+      </c>
+      <c r="P15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.79424241351634539</v>
+      </c>
+      <c r="Q15" s="2">
+        <f t="shared" si="0"/>
+        <v>0.8781245256710698</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
@@ -890,6 +1221,39 @@
       <c r="D16">
         <v>1017</v>
       </c>
+      <c r="E16">
+        <v>215</v>
+      </c>
+      <c r="F16">
+        <v>40651530</v>
+      </c>
+      <c r="G16">
+        <v>23065000</v>
+      </c>
+      <c r="H16">
+        <v>13510000</v>
+      </c>
+      <c r="I16">
+        <v>110711328</v>
+      </c>
+      <c r="J16">
+        <v>109950650</v>
+      </c>
+      <c r="K16">
+        <v>110663296</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="1"/>
+        <v>0.63281508103669393</v>
+      </c>
+      <c r="P16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7902240687071882</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.87791796839306147</v>
+      </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -904,6 +1268,39 @@
       <c r="D17">
         <v>963</v>
       </c>
+      <c r="E17">
+        <v>230</v>
+      </c>
+      <c r="F17">
+        <v>42394191</v>
+      </c>
+      <c r="G17">
+        <v>22790755</v>
+      </c>
+      <c r="H17">
+        <v>13580000</v>
+      </c>
+      <c r="I17">
+        <v>116183024</v>
+      </c>
+      <c r="J17">
+        <v>116153232</v>
+      </c>
+      <c r="K17">
+        <v>116138640</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="1"/>
+        <v>0.63510855940537403</v>
+      </c>
+      <c r="P17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.80378716452763022</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.88307078505482761</v>
+      </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -918,6 +1315,42 @@
       <c r="D18">
         <v>1179</v>
       </c>
+      <c r="E18">
+        <v>192</v>
+      </c>
+      <c r="F18">
+        <v>53158942</v>
+      </c>
+      <c r="G18">
+        <v>28445340</v>
+      </c>
+      <c r="H18">
+        <v>16555000</v>
+      </c>
+      <c r="I18">
+        <v>137836336</v>
+      </c>
+      <c r="J18">
+        <v>136893278</v>
+      </c>
+      <c r="K18">
+        <v>137782224</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.61433288534309272</v>
+      </c>
+      <c r="P18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7922079125024678</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.87984661940135322</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="O19" s="2"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
@@ -962,6 +1395,9 @@
       <c r="D21" t="s">
         <v>25</v>
       </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
       <c r="F21" t="s">
         <v>1</v>
       </c>
@@ -1021,8 +1457,38 @@
       <c r="D22">
         <v>475</v>
       </c>
+      <c r="E22">
+        <v>177</v>
+      </c>
       <c r="F22">
-        <v>2730000</v>
+        <v>2905000</v>
+      </c>
+      <c r="G22">
+        <v>2905000</v>
+      </c>
+      <c r="H22">
+        <v>3325000</v>
+      </c>
+      <c r="I22">
+        <v>327672</v>
+      </c>
+      <c r="J22">
+        <v>313720</v>
+      </c>
+      <c r="K22">
+        <v>928098</v>
+      </c>
+      <c r="O22" s="3">
+        <f>I22/F22</f>
+        <v>0.11279586919104992</v>
+      </c>
+      <c r="P22" s="3">
+        <f t="shared" ref="P22:Q35" si="2">J22/G22</f>
+        <v>0.10799311531841653</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="2"/>
+        <v>0.27912721804511276</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -1038,8 +1504,38 @@
       <c r="D23">
         <v>433</v>
       </c>
+      <c r="E23">
+        <v>154</v>
+      </c>
       <c r="F23">
-        <v>2975000</v>
+        <v>2765000</v>
+      </c>
+      <c r="G23">
+        <v>2765000</v>
+      </c>
+      <c r="H23">
+        <v>2765000</v>
+      </c>
+      <c r="I23">
+        <v>340720</v>
+      </c>
+      <c r="J23">
+        <v>340684</v>
+      </c>
+      <c r="K23">
+        <v>681352</v>
+      </c>
+      <c r="O23" s="3">
+        <f t="shared" ref="O23:O35" si="3">I23/F23</f>
+        <v>0.12322603978300181</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.12321301989150091</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.24642025316455696</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
@@ -1055,8 +1551,38 @@
       <c r="D24">
         <v>421</v>
       </c>
+      <c r="E24">
+        <v>118</v>
+      </c>
       <c r="F24">
-        <v>2351700</v>
+        <v>2141100</v>
+      </c>
+      <c r="G24">
+        <v>2221050</v>
+      </c>
+      <c r="H24">
+        <v>2252364</v>
+      </c>
+      <c r="I24">
+        <v>705600</v>
+      </c>
+      <c r="J24">
+        <v>705240</v>
+      </c>
+      <c r="K24">
+        <v>705126</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" si="3"/>
+        <v>0.32955023118957544</v>
+      </c>
+      <c r="P24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.31752549469845343</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.31306041119463818</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
@@ -1072,8 +1598,38 @@
       <c r="D25">
         <v>1471</v>
       </c>
+      <c r="E25">
+        <v>440</v>
+      </c>
       <c r="F25">
-        <v>3525285</v>
+        <v>3596145</v>
+      </c>
+      <c r="G25">
+        <v>3596145</v>
+      </c>
+      <c r="H25">
+        <v>3596145</v>
+      </c>
+      <c r="I25">
+        <v>381237</v>
+      </c>
+      <c r="J25">
+        <v>380833</v>
+      </c>
+      <c r="K25">
+        <v>380651</v>
+      </c>
+      <c r="O25" s="3">
+        <f t="shared" si="3"/>
+        <v>0.10601268858736231</v>
+      </c>
+      <c r="P25" s="3">
+        <f t="shared" si="2"/>
+        <v>0.10590034606502241</v>
+      </c>
+      <c r="Q25" s="3">
+        <f t="shared" si="2"/>
+        <v>0.10584973631485939</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
@@ -1089,8 +1645,38 @@
       <c r="D26">
         <v>197</v>
       </c>
+      <c r="E26">
+        <v>117</v>
+      </c>
       <c r="F26">
-        <v>53988</v>
+        <v>53170</v>
+      </c>
+      <c r="G26">
+        <v>53170</v>
+      </c>
+      <c r="H26">
+        <v>55624</v>
+      </c>
+      <c r="I26">
+        <v>9498</v>
+      </c>
+      <c r="J26">
+        <v>9486</v>
+      </c>
+      <c r="K26">
+        <v>9484</v>
+      </c>
+      <c r="O26" s="3">
+        <f t="shared" si="3"/>
+        <v>0.17863456836561972</v>
+      </c>
+      <c r="P26" s="3">
+        <f t="shared" si="2"/>
+        <v>0.17840887718638329</v>
+      </c>
+      <c r="Q26" s="3">
+        <f t="shared" si="2"/>
+        <v>0.17050194160793902</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
@@ -1106,8 +1692,38 @@
       <c r="D27">
         <v>2542</v>
       </c>
+      <c r="E27">
+        <v>235</v>
+      </c>
       <c r="F27">
-        <v>4894032</v>
+        <v>5091372</v>
+      </c>
+      <c r="G27">
+        <v>4546688</v>
+      </c>
+      <c r="H27">
+        <v>4585000</v>
+      </c>
+      <c r="I27">
+        <v>644670</v>
+      </c>
+      <c r="J27">
+        <v>1222128</v>
+      </c>
+      <c r="K27">
+        <v>1219424</v>
+      </c>
+      <c r="O27" s="3">
+        <f t="shared" si="3"/>
+        <v>0.12662009375861752</v>
+      </c>
+      <c r="P27" s="3">
+        <f t="shared" si="2"/>
+        <v>0.26879521972917431</v>
+      </c>
+      <c r="Q27" s="3">
+        <f t="shared" si="2"/>
+        <v>0.26595943293347873</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
@@ -1123,8 +1739,38 @@
       <c r="D28">
         <v>89</v>
       </c>
+      <c r="E28">
+        <v>68</v>
+      </c>
       <c r="F28">
         <v>2443840</v>
+      </c>
+      <c r="G28">
+        <v>2443840</v>
+      </c>
+      <c r="H28">
+        <v>2443840</v>
+      </c>
+      <c r="I28">
+        <v>374552</v>
+      </c>
+      <c r="J28">
+        <v>1123452</v>
+      </c>
+      <c r="K28">
+        <v>1123452</v>
+      </c>
+      <c r="O28" s="3">
+        <f t="shared" si="3"/>
+        <v>0.15326371611889486</v>
+      </c>
+      <c r="P28" s="3">
+        <f t="shared" si="2"/>
+        <v>0.45970767317009298</v>
+      </c>
+      <c r="Q28" s="3">
+        <f t="shared" si="2"/>
+        <v>0.45970767317009298</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
@@ -1140,6 +1786,39 @@
       <c r="D29">
         <v>909</v>
       </c>
+      <c r="E29">
+        <v>189</v>
+      </c>
+      <c r="F29">
+        <v>3080000</v>
+      </c>
+      <c r="G29">
+        <v>3080000</v>
+      </c>
+      <c r="H29">
+        <v>3500000</v>
+      </c>
+      <c r="I29">
+        <v>1762338</v>
+      </c>
+      <c r="J29">
+        <v>1761774</v>
+      </c>
+      <c r="K29">
+        <v>1761498</v>
+      </c>
+      <c r="O29" s="3">
+        <f t="shared" si="3"/>
+        <v>0.57218766233766238</v>
+      </c>
+      <c r="P29" s="3">
+        <f t="shared" si="2"/>
+        <v>0.57200454545454549</v>
+      </c>
+      <c r="Q29" s="3">
+        <f t="shared" si="2"/>
+        <v>0.50328514285714288</v>
+      </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
@@ -1154,6 +1833,39 @@
       <c r="D30">
         <v>747</v>
       </c>
+      <c r="E30">
+        <v>190</v>
+      </c>
+      <c r="F30">
+        <v>3653574</v>
+      </c>
+      <c r="G30">
+        <v>3395000</v>
+      </c>
+      <c r="H30">
+        <v>3395000</v>
+      </c>
+      <c r="I30">
+        <v>1444164</v>
+      </c>
+      <c r="J30">
+        <v>962432</v>
+      </c>
+      <c r="K30">
+        <v>1443414</v>
+      </c>
+      <c r="O30" s="3">
+        <f t="shared" si="3"/>
+        <v>0.39527432590663281</v>
+      </c>
+      <c r="P30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.28348512518409424</v>
+      </c>
+      <c r="Q30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.42515876288659793</v>
+      </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1168,6 +1880,39 @@
       <c r="D31">
         <v>855</v>
       </c>
+      <c r="E31">
+        <v>200</v>
+      </c>
+      <c r="F31">
+        <v>3605000</v>
+      </c>
+      <c r="G31">
+        <v>3605000</v>
+      </c>
+      <c r="H31">
+        <v>3605000</v>
+      </c>
+      <c r="I31">
+        <v>1850118</v>
+      </c>
+      <c r="J31">
+        <v>1233040</v>
+      </c>
+      <c r="K31">
+        <v>1849296</v>
+      </c>
+      <c r="O31" s="3">
+        <f t="shared" si="3"/>
+        <v>0.51320887656033287</v>
+      </c>
+      <c r="P31" s="3">
+        <f t="shared" si="2"/>
+        <v>0.34203606102635231</v>
+      </c>
+      <c r="Q31" s="3">
+        <f t="shared" si="2"/>
+        <v>0.51298085991678222</v>
+      </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -1182,6 +1927,39 @@
       <c r="D32">
         <v>1017</v>
       </c>
+      <c r="E32">
+        <v>215</v>
+      </c>
+      <c r="F32">
+        <v>3979128</v>
+      </c>
+      <c r="G32">
+        <v>3885000</v>
+      </c>
+      <c r="H32">
+        <v>3885000</v>
+      </c>
+      <c r="I32">
+        <v>1933734</v>
+      </c>
+      <c r="J32">
+        <v>1288728</v>
+      </c>
+      <c r="K32">
+        <v>1932786</v>
+      </c>
+      <c r="O32" s="3">
+        <f t="shared" si="3"/>
+        <v>0.48596928774344528</v>
+      </c>
+      <c r="P32" s="3">
+        <f t="shared" si="2"/>
+        <v>0.33171891891891891</v>
+      </c>
+      <c r="Q32" s="3">
+        <f t="shared" si="2"/>
+        <v>0.49749961389961389</v>
+      </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
@@ -1196,6 +1974,39 @@
       <c r="D33">
         <v>1017</v>
       </c>
+      <c r="E33">
+        <v>215</v>
+      </c>
+      <c r="F33">
+        <v>4065153</v>
+      </c>
+      <c r="G33">
+        <v>3990000</v>
+      </c>
+      <c r="H33">
+        <v>3990000</v>
+      </c>
+      <c r="I33">
+        <v>2185092</v>
+      </c>
+      <c r="J33">
+        <v>1456300</v>
+      </c>
+      <c r="K33">
+        <v>2184144</v>
+      </c>
+      <c r="O33" s="3">
+        <f t="shared" si="3"/>
+        <v>0.53751777608370455</v>
+      </c>
+      <c r="P33" s="3">
+        <f t="shared" si="2"/>
+        <v>0.36498746867167919</v>
+      </c>
+      <c r="Q33" s="3">
+        <f t="shared" si="2"/>
+        <v>0.54740451127819545</v>
+      </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1210,6 +2021,39 @@
       <c r="D34">
         <v>963</v>
       </c>
+      <c r="E34">
+        <v>230</v>
+      </c>
+      <c r="F34">
+        <v>3645978</v>
+      </c>
+      <c r="G34">
+        <v>3413280</v>
+      </c>
+      <c r="H34">
+        <v>3605000</v>
+      </c>
+      <c r="I34">
+        <v>2293086</v>
+      </c>
+      <c r="J34">
+        <v>2292498</v>
+      </c>
+      <c r="K34">
+        <v>2292210</v>
+      </c>
+      <c r="O34" s="3">
+        <f t="shared" si="3"/>
+        <v>0.62893577525700928</v>
+      </c>
+      <c r="P34" s="3">
+        <f t="shared" si="2"/>
+        <v>0.67164076782449722</v>
+      </c>
+      <c r="Q34" s="3">
+        <f t="shared" si="2"/>
+        <v>0.63584188626907079</v>
+      </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
@@ -1223,6 +2067,39 @@
       </c>
       <c r="D35">
         <v>1179</v>
+      </c>
+      <c r="E35">
+        <v>192</v>
+      </c>
+      <c r="F35">
+        <v>4945953</v>
+      </c>
+      <c r="G35">
+        <v>4342800</v>
+      </c>
+      <c r="H35">
+        <v>4235000</v>
+      </c>
+      <c r="I35">
+        <v>2720454</v>
+      </c>
+      <c r="J35">
+        <v>1813156</v>
+      </c>
+      <c r="K35">
+        <v>2719386</v>
+      </c>
+      <c r="O35" s="3">
+        <f t="shared" si="3"/>
+        <v>0.55003636306289205</v>
+      </c>
+      <c r="P35" s="3">
+        <f t="shared" si="2"/>
+        <v>0.41750851984894538</v>
+      </c>
+      <c r="Q35" s="3">
+        <f t="shared" si="2"/>
+        <v>0.6421218417945691</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
@@ -1268,6 +2145,9 @@
       <c r="D38" t="s">
         <v>25</v>
       </c>
+      <c r="E38" t="s">
+        <v>38</v>
+      </c>
       <c r="F38" t="s">
         <v>1</v>
       </c>
@@ -1327,8 +2207,38 @@
       <c r="D39">
         <v>475</v>
       </c>
+      <c r="E39">
+        <v>177</v>
+      </c>
       <c r="F39">
-        <v>78</v>
+        <v>83</v>
+      </c>
+      <c r="G39">
+        <v>83</v>
+      </c>
+      <c r="H39">
+        <v>95</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="J39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <v>3</v>
+      </c>
+      <c r="O39" s="3">
+        <f>I39/F39</f>
+        <v>1.2048192771084338E-2</v>
+      </c>
+      <c r="P39" s="3">
+        <f t="shared" ref="P39:Q39" si="4">J39/G39</f>
+        <v>1.2048192771084338E-2</v>
+      </c>
+      <c r="Q39" s="3">
+        <f t="shared" si="4"/>
+        <v>3.1578947368421054E-2</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
@@ -1344,8 +2254,38 @@
       <c r="D40">
         <v>433</v>
       </c>
+      <c r="E40">
+        <v>154</v>
+      </c>
       <c r="F40">
-        <v>85</v>
+        <v>79</v>
+      </c>
+      <c r="G40">
+        <v>79</v>
+      </c>
+      <c r="H40">
+        <v>79</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="J40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <v>2</v>
+      </c>
+      <c r="O40" s="3">
+        <f t="shared" ref="O40:O52" si="5">I40/F40</f>
+        <v>1.2658227848101266E-2</v>
+      </c>
+      <c r="P40" s="3">
+        <f t="shared" ref="P40:P52" si="6">J40/G40</f>
+        <v>1.2658227848101266E-2</v>
+      </c>
+      <c r="Q40" s="3">
+        <f t="shared" ref="Q40:Q52" si="7">K40/H40</f>
+        <v>2.5316455696202531E-2</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
@@ -1361,8 +2301,38 @@
       <c r="D41">
         <v>421</v>
       </c>
+      <c r="E41">
+        <v>118</v>
+      </c>
       <c r="F41">
+        <v>61</v>
+      </c>
+      <c r="G41">
         <v>67</v>
+      </c>
+      <c r="H41">
+        <v>68</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>3</v>
+      </c>
+      <c r="K41">
+        <v>3</v>
+      </c>
+      <c r="O41" s="3">
+        <f t="shared" si="5"/>
+        <v>4.9180327868852458E-2</v>
+      </c>
+      <c r="P41" s="3">
+        <f t="shared" si="6"/>
+        <v>4.4776119402985072E-2</v>
+      </c>
+      <c r="Q41" s="3">
+        <f t="shared" si="7"/>
+        <v>4.4117647058823532E-2</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
@@ -1378,8 +2348,38 @@
       <c r="D42">
         <v>1471</v>
       </c>
+      <c r="E42">
+        <v>440</v>
+      </c>
       <c r="F42">
-        <v>199</v>
+        <v>203</v>
+      </c>
+      <c r="G42">
+        <v>203</v>
+      </c>
+      <c r="H42">
+        <v>203</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="O42" s="3">
+        <f t="shared" si="5"/>
+        <v>4.9261083743842365E-3</v>
+      </c>
+      <c r="P42" s="3">
+        <f t="shared" si="6"/>
+        <v>4.9261083743842365E-3</v>
+      </c>
+      <c r="Q42" s="3">
+        <f t="shared" si="7"/>
+        <v>4.9261083743842365E-3</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
@@ -1395,8 +2395,38 @@
       <c r="D43">
         <v>197</v>
       </c>
+      <c r="E43">
+        <v>117</v>
+      </c>
       <c r="F43">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="G43">
+        <v>65</v>
+      </c>
+      <c r="H43">
+        <v>68</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="O43" s="3">
+        <f t="shared" si="5"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="P43" s="3">
+        <f t="shared" si="6"/>
+        <v>1.5384615384615385E-2</v>
+      </c>
+      <c r="Q43" s="3">
+        <f t="shared" si="7"/>
+        <v>1.4705882352941176E-2</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
@@ -1416,7 +2446,34 @@
         <v>235</v>
       </c>
       <c r="F44">
-        <v>124</v>
+        <v>129</v>
+      </c>
+      <c r="G44">
+        <v>128</v>
+      </c>
+      <c r="H44">
+        <v>131</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <v>2</v>
+      </c>
+      <c r="K44">
+        <v>2</v>
+      </c>
+      <c r="O44" s="3">
+        <f t="shared" si="5"/>
+        <v>7.7519379844961239E-3</v>
+      </c>
+      <c r="P44" s="3">
+        <f t="shared" si="6"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="Q44" s="3">
+        <f t="shared" si="7"/>
+        <v>1.5267175572519083E-2</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
@@ -1432,8 +2489,38 @@
       <c r="D45">
         <v>89</v>
       </c>
+      <c r="E45">
+        <v>68</v>
+      </c>
       <c r="F45">
         <v>40</v>
+      </c>
+      <c r="G45">
+        <v>40</v>
+      </c>
+      <c r="H45">
+        <v>40</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="O45" s="3">
+        <f t="shared" si="5"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P45" s="3">
+        <f t="shared" si="6"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="Q45" s="3">
+        <f t="shared" si="7"/>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
@@ -1449,6 +2536,39 @@
       <c r="D46">
         <v>909</v>
       </c>
+      <c r="E46">
+        <v>189</v>
+      </c>
+      <c r="F46">
+        <v>88</v>
+      </c>
+      <c r="G46">
+        <v>88</v>
+      </c>
+      <c r="H46">
+        <v>100</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="J46">
+        <v>3</v>
+      </c>
+      <c r="K46">
+        <v>3</v>
+      </c>
+      <c r="O46" s="3">
+        <f t="shared" si="5"/>
+        <v>3.4090909090909088E-2</v>
+      </c>
+      <c r="P46" s="3">
+        <f t="shared" si="6"/>
+        <v>3.4090909090909088E-2</v>
+      </c>
+      <c r="Q46" s="3">
+        <f t="shared" si="7"/>
+        <v>0.03</v>
+      </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -1463,6 +2583,39 @@
       <c r="D47">
         <v>747</v>
       </c>
+      <c r="E47">
+        <v>190</v>
+      </c>
+      <c r="F47">
+        <v>101</v>
+      </c>
+      <c r="G47">
+        <v>97</v>
+      </c>
+      <c r="H47">
+        <v>97</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>3</v>
+      </c>
+      <c r="O47" s="3">
+        <f t="shared" si="5"/>
+        <v>2.9702970297029702E-2</v>
+      </c>
+      <c r="P47" s="3">
+        <f t="shared" si="6"/>
+        <v>2.0618556701030927E-2</v>
+      </c>
+      <c r="Q47" s="3">
+        <f t="shared" si="7"/>
+        <v>3.0927835051546393E-2</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
@@ -1477,6 +2630,39 @@
       <c r="D48">
         <v>855</v>
       </c>
+      <c r="E48">
+        <v>200</v>
+      </c>
+      <c r="F48">
+        <v>103</v>
+      </c>
+      <c r="G48">
+        <v>103</v>
+      </c>
+      <c r="H48">
+        <v>103</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="O48" s="3">
+        <f t="shared" si="5"/>
+        <v>2.9126213592233011E-2</v>
+      </c>
+      <c r="P48" s="3">
+        <f t="shared" si="6"/>
+        <v>1.9417475728155338E-2</v>
+      </c>
+      <c r="Q48" s="3">
+        <f t="shared" si="7"/>
+        <v>2.9126213592233011E-2</v>
+      </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
@@ -1491,6 +2677,39 @@
       <c r="D49">
         <v>1017</v>
       </c>
+      <c r="E49">
+        <v>215</v>
+      </c>
+      <c r="F49">
+        <v>111</v>
+      </c>
+      <c r="G49">
+        <v>111</v>
+      </c>
+      <c r="H49">
+        <v>111</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>3</v>
+      </c>
+      <c r="O49" s="3">
+        <f t="shared" si="5"/>
+        <v>2.7027027027027029E-2</v>
+      </c>
+      <c r="P49" s="3">
+        <f t="shared" si="6"/>
+        <v>1.8018018018018018E-2</v>
+      </c>
+      <c r="Q49" s="3">
+        <f t="shared" si="7"/>
+        <v>2.7027027027027029E-2</v>
+      </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
@@ -1505,6 +2724,39 @@
       <c r="D50">
         <v>1017</v>
       </c>
+      <c r="E50">
+        <v>215</v>
+      </c>
+      <c r="F50">
+        <v>111</v>
+      </c>
+      <c r="G50">
+        <v>114</v>
+      </c>
+      <c r="H50">
+        <v>114</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="O50" s="3">
+        <f t="shared" si="5"/>
+        <v>2.7027027027027029E-2</v>
+      </c>
+      <c r="P50" s="3">
+        <f t="shared" si="6"/>
+        <v>1.7543859649122806E-2</v>
+      </c>
+      <c r="Q50" s="3">
+        <f t="shared" si="7"/>
+        <v>2.6315789473684209E-2</v>
+      </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
@@ -1519,6 +2771,39 @@
       <c r="D51">
         <v>963</v>
       </c>
+      <c r="E51">
+        <v>230</v>
+      </c>
+      <c r="F51">
+        <v>94</v>
+      </c>
+      <c r="G51">
+        <v>96</v>
+      </c>
+      <c r="H51">
+        <v>103</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>3</v>
+      </c>
+      <c r="K51">
+        <v>3</v>
+      </c>
+      <c r="O51" s="3">
+        <f t="shared" si="5"/>
+        <v>3.1914893617021274E-2</v>
+      </c>
+      <c r="P51" s="3">
+        <f t="shared" si="6"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="Q51" s="3">
+        <f t="shared" si="7"/>
+        <v>2.9126213592233011E-2</v>
+      </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
@@ -1532,6 +2817,39 @@
       </c>
       <c r="D52">
         <v>1179</v>
+      </c>
+      <c r="E52">
+        <v>192</v>
+      </c>
+      <c r="F52">
+        <v>123</v>
+      </c>
+      <c r="G52">
+        <v>120</v>
+      </c>
+      <c r="H52">
+        <v>121</v>
+      </c>
+      <c r="I52">
+        <v>3</v>
+      </c>
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="K52">
+        <v>3</v>
+      </c>
+      <c r="O52" s="3">
+        <f t="shared" si="5"/>
+        <v>2.4390243902439025E-2</v>
+      </c>
+      <c r="P52" s="3">
+        <f t="shared" si="6"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="Q52" s="3">
+        <f t="shared" si="7"/>
+        <v>2.4793388429752067E-2</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
@@ -1577,6 +2895,9 @@
       <c r="D55" t="s">
         <v>25</v>
       </c>
+      <c r="E55" t="s">
+        <v>38</v>
+      </c>
       <c r="F55" t="s">
         <v>1</v>
       </c>
@@ -1636,8 +2957,38 @@
       <c r="D56">
         <v>475</v>
       </c>
+      <c r="E56">
+        <v>177</v>
+      </c>
       <c r="F56">
-        <v>12804904</v>
+        <v>14022000</v>
+      </c>
+      <c r="G56">
+        <v>14022000</v>
+      </c>
+      <c r="H56">
+        <v>14202740</v>
+      </c>
+      <c r="I56">
+        <v>18155400</v>
+      </c>
+      <c r="J56">
+        <v>18807600</v>
+      </c>
+      <c r="K56">
+        <v>18868200</v>
+      </c>
+      <c r="O56" s="3">
+        <f>I56/F56</f>
+        <v>1.2947796320068463</v>
+      </c>
+      <c r="P56" s="3">
+        <f t="shared" ref="P56:Q56" si="8">J56/G56</f>
+        <v>1.3412922550278135</v>
+      </c>
+      <c r="Q56" s="3">
+        <f t="shared" si="8"/>
+        <v>1.3284901364102983</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
@@ -1653,8 +3004,38 @@
       <c r="D57">
         <v>433</v>
       </c>
+      <c r="E57">
+        <v>154</v>
+      </c>
       <c r="F57">
-        <v>12008752</v>
+        <v>12879600</v>
+      </c>
+      <c r="G57">
+        <v>12879600</v>
+      </c>
+      <c r="H57">
+        <v>12879600</v>
+      </c>
+      <c r="I57">
+        <v>16204800</v>
+      </c>
+      <c r="J57">
+        <v>16738200</v>
+      </c>
+      <c r="K57">
+        <v>16909800</v>
+      </c>
+      <c r="O57" s="3">
+        <f t="shared" ref="O57:O69" si="9">I57/F57</f>
+        <v>1.2581757197428491</v>
+      </c>
+      <c r="P57" s="3">
+        <f t="shared" ref="P57:P69" si="10">J57/G57</f>
+        <v>1.2995900493804156</v>
+      </c>
+      <c r="Q57" s="3">
+        <f t="shared" ref="Q57:Q69" si="11">K57/H57</f>
+        <v>1.3129134445169104</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
@@ -1670,8 +3051,38 @@
       <c r="D58">
         <v>421</v>
       </c>
+      <c r="E58">
+        <v>118</v>
+      </c>
       <c r="F58">
-        <v>12432888</v>
+        <v>12776385</v>
+      </c>
+      <c r="G58">
+        <v>12681878</v>
+      </c>
+      <c r="H58">
+        <v>12775672</v>
+      </c>
+      <c r="I58">
+        <v>16106148</v>
+      </c>
+      <c r="J58">
+        <v>16278826</v>
+      </c>
+      <c r="K58">
+        <v>16690648</v>
+      </c>
+      <c r="O58" s="3">
+        <f t="shared" si="9"/>
+        <v>1.2606185552486091</v>
+      </c>
+      <c r="P58" s="3">
+        <f t="shared" si="10"/>
+        <v>1.2836289704095876</v>
+      </c>
+      <c r="Q58" s="3">
+        <f t="shared" si="11"/>
+        <v>1.30643992738699</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
@@ -1687,8 +3098,38 @@
       <c r="D59">
         <v>1471</v>
       </c>
+      <c r="E59">
+        <v>440</v>
+      </c>
       <c r="F59">
-        <v>48813436</v>
+        <v>49188000</v>
+      </c>
+      <c r="G59">
+        <v>49188000</v>
+      </c>
+      <c r="H59">
+        <v>49188000</v>
+      </c>
+      <c r="I59">
+        <v>64633000</v>
+      </c>
+      <c r="J59">
+        <v>65572000</v>
+      </c>
+      <c r="K59">
+        <v>64226000</v>
+      </c>
+      <c r="O59" s="3">
+        <f t="shared" si="9"/>
+        <v>1.3139993494348214</v>
+      </c>
+      <c r="P59" s="3">
+        <f t="shared" si="10"/>
+        <v>1.3330893713913963</v>
+      </c>
+      <c r="Q59" s="3">
+        <f t="shared" si="11"/>
+        <v>1.3057249735707896</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
@@ -1704,8 +3145,38 @@
       <c r="D60">
         <v>197</v>
       </c>
+      <c r="E60">
+        <v>117</v>
+      </c>
       <c r="F60">
-        <v>7215083</v>
+        <v>7311018</v>
+      </c>
+      <c r="G60">
+        <v>7311018</v>
+      </c>
+      <c r="H60">
+        <v>7302641</v>
+      </c>
+      <c r="I60">
+        <v>9867000</v>
+      </c>
+      <c r="J60">
+        <v>10149000</v>
+      </c>
+      <c r="K60">
+        <v>9985778</v>
+      </c>
+      <c r="O60" s="3">
+        <f t="shared" si="9"/>
+        <v>1.3496068536556742</v>
+      </c>
+      <c r="P60" s="3">
+        <f t="shared" si="10"/>
+        <v>1.3881787734621909</v>
+      </c>
+      <c r="Q60" s="3">
+        <f t="shared" si="11"/>
+        <v>1.3674200881571474</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
@@ -1721,8 +3192,38 @@
       <c r="D61">
         <v>2542</v>
       </c>
+      <c r="E61">
+        <v>235</v>
+      </c>
       <c r="F61">
-        <v>62780839</v>
+        <v>62880000</v>
+      </c>
+      <c r="G61">
+        <v>64558930</v>
+      </c>
+      <c r="H61">
+        <v>66306108</v>
+      </c>
+      <c r="I61">
+        <v>84848400</v>
+      </c>
+      <c r="J61">
+        <v>87228000</v>
+      </c>
+      <c r="K61">
+        <v>87875400</v>
+      </c>
+      <c r="O61" s="3">
+        <f t="shared" si="9"/>
+        <v>1.3493702290076335</v>
+      </c>
+      <c r="P61" s="3">
+        <f t="shared" si="10"/>
+        <v>1.3511376350258593</v>
+      </c>
+      <c r="Q61" s="3">
+        <f t="shared" si="11"/>
+        <v>1.3252987190863321</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
@@ -1738,8 +3239,38 @@
       <c r="D62">
         <v>89</v>
       </c>
+      <c r="E62">
+        <v>68</v>
+      </c>
       <c r="F62">
-        <v>3829602</v>
+        <v>4139200</v>
+      </c>
+      <c r="G62">
+        <v>4226056</v>
+      </c>
+      <c r="H62">
+        <v>4234330</v>
+      </c>
+      <c r="I62">
+        <v>5373543</v>
+      </c>
+      <c r="J62">
+        <v>5299771</v>
+      </c>
+      <c r="K62">
+        <v>5524347</v>
+      </c>
+      <c r="O62" s="3">
+        <f t="shared" si="9"/>
+        <v>1.298208107846927</v>
+      </c>
+      <c r="P62" s="3">
+        <f t="shared" si="10"/>
+        <v>1.25407022528807</v>
+      </c>
+      <c r="Q62" s="3">
+        <f t="shared" si="11"/>
+        <v>1.3046566989346602</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
@@ -1755,6 +3286,39 @@
       <c r="D63">
         <v>909</v>
       </c>
+      <c r="E63">
+        <v>189</v>
+      </c>
+      <c r="F63">
+        <v>23094000</v>
+      </c>
+      <c r="G63">
+        <v>23094000</v>
+      </c>
+      <c r="H63">
+        <v>23787698</v>
+      </c>
+      <c r="I63">
+        <v>28914600</v>
+      </c>
+      <c r="J63">
+        <v>30617400</v>
+      </c>
+      <c r="K63">
+        <v>29916600</v>
+      </c>
+      <c r="O63" s="3">
+        <f t="shared" si="9"/>
+        <v>1.2520394907768251</v>
+      </c>
+      <c r="P63" s="3">
+        <f t="shared" si="10"/>
+        <v>1.3257729280332553</v>
+      </c>
+      <c r="Q63" s="3">
+        <f t="shared" si="11"/>
+        <v>1.2576500676946547</v>
+      </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
@@ -1769,6 +3333,39 @@
       <c r="D64">
         <v>747</v>
       </c>
+      <c r="E64">
+        <v>190</v>
+      </c>
+      <c r="F64">
+        <v>20019338</v>
+      </c>
+      <c r="G64">
+        <v>20420344</v>
+      </c>
+      <c r="H64">
+        <v>20478192</v>
+      </c>
+      <c r="I64">
+        <v>25359000</v>
+      </c>
+      <c r="J64">
+        <v>26887800</v>
+      </c>
+      <c r="K64">
+        <v>25185000</v>
+      </c>
+      <c r="O64" s="3">
+        <f t="shared" si="9"/>
+        <v>1.2667252034008318</v>
+      </c>
+      <c r="P64" s="3">
+        <f t="shared" si="10"/>
+        <v>1.3167163099700965</v>
+      </c>
+      <c r="Q64" s="3">
+        <f t="shared" si="11"/>
+        <v>1.2298449003701108</v>
+      </c>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
@@ -1783,6 +3380,39 @@
       <c r="D65">
         <v>855</v>
       </c>
+      <c r="E65">
+        <v>200</v>
+      </c>
+      <c r="F65">
+        <v>22876854</v>
+      </c>
+      <c r="G65">
+        <v>22876854</v>
+      </c>
+      <c r="H65">
+        <v>22930180</v>
+      </c>
+      <c r="I65">
+        <v>28418400</v>
+      </c>
+      <c r="J65">
+        <v>29710800</v>
+      </c>
+      <c r="K65">
+        <v>28620600</v>
+      </c>
+      <c r="O65" s="3">
+        <f t="shared" si="9"/>
+        <v>1.2422337442027649</v>
+      </c>
+      <c r="P65" s="3">
+        <f t="shared" si="10"/>
+        <v>1.2987275260837876</v>
+      </c>
+      <c r="Q65" s="3">
+        <f t="shared" si="11"/>
+        <v>1.2481629014687194</v>
+      </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
@@ -1797,6 +3427,39 @@
       <c r="D66">
         <v>1017</v>
       </c>
+      <c r="E66">
+        <v>215</v>
+      </c>
+      <c r="F66">
+        <v>26193882</v>
+      </c>
+      <c r="G66">
+        <v>26888400</v>
+      </c>
+      <c r="H66">
+        <v>26887476</v>
+      </c>
+      <c r="I66">
+        <v>32819400</v>
+      </c>
+      <c r="J66">
+        <v>34914600</v>
+      </c>
+      <c r="K66">
+        <v>35985000</v>
+      </c>
+      <c r="O66" s="3">
+        <f t="shared" si="9"/>
+        <v>1.2529414311326592</v>
+      </c>
+      <c r="P66" s="3">
+        <f t="shared" si="10"/>
+        <v>1.2985004686035615</v>
+      </c>
+      <c r="Q66" s="3">
+        <f t="shared" si="11"/>
+        <v>1.338355448462325</v>
+      </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
@@ -1811,6 +3474,39 @@
       <c r="D67">
         <v>1017</v>
       </c>
+      <c r="E67">
+        <v>215</v>
+      </c>
+      <c r="F67">
+        <v>25360000</v>
+      </c>
+      <c r="G67">
+        <v>26499564</v>
+      </c>
+      <c r="H67">
+        <v>26499564</v>
+      </c>
+      <c r="I67">
+        <v>32641800</v>
+      </c>
+      <c r="J67">
+        <v>34147800</v>
+      </c>
+      <c r="K67">
+        <v>33622200</v>
+      </c>
+      <c r="O67" s="3">
+        <f t="shared" si="9"/>
+        <v>1.2871372239747634</v>
+      </c>
+      <c r="P67" s="3">
+        <f t="shared" si="10"/>
+        <v>1.2886174278188125</v>
+      </c>
+      <c r="Q67" s="3">
+        <f t="shared" si="11"/>
+        <v>1.2687831392244793</v>
+      </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
@@ -1825,6 +3521,39 @@
       <c r="D68">
         <v>963</v>
       </c>
+      <c r="E68">
+        <v>230</v>
+      </c>
+      <c r="F68">
+        <v>23656000</v>
+      </c>
+      <c r="G68">
+        <v>24315564</v>
+      </c>
+      <c r="H68">
+        <v>24562252</v>
+      </c>
+      <c r="I68">
+        <v>30824400</v>
+      </c>
+      <c r="J68">
+        <v>31810800</v>
+      </c>
+      <c r="K68">
+        <v>33671400</v>
+      </c>
+      <c r="O68" s="3">
+        <f t="shared" si="9"/>
+        <v>1.3030267162664864</v>
+      </c>
+      <c r="P68" s="3">
+        <f t="shared" si="10"/>
+        <v>1.3082484946678596</v>
+      </c>
+      <c r="Q68" s="3">
+        <f t="shared" si="11"/>
+        <v>1.3708596426744584</v>
+      </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
@@ -1838,6 +3567,39 @@
       </c>
       <c r="D69">
         <v>1179</v>
+      </c>
+      <c r="E69">
+        <v>192</v>
+      </c>
+      <c r="F69">
+        <v>29749200</v>
+      </c>
+      <c r="G69">
+        <v>29130558</v>
+      </c>
+      <c r="H69">
+        <v>29901218</v>
+      </c>
+      <c r="I69">
+        <v>37382400</v>
+      </c>
+      <c r="J69">
+        <v>39082200</v>
+      </c>
+      <c r="K69">
+        <v>36964800</v>
+      </c>
+      <c r="O69" s="3">
+        <f t="shared" si="9"/>
+        <v>1.2565850510265821</v>
+      </c>
+      <c r="P69" s="3">
+        <f t="shared" si="10"/>
+        <v>1.3416220863328467</v>
+      </c>
+      <c r="Q69" s="3">
+        <f t="shared" si="11"/>
+        <v>1.2362305776306504</v>
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.2">
@@ -1883,6 +3645,9 @@
       <c r="D72" t="s">
         <v>25</v>
       </c>
+      <c r="E72" t="s">
+        <v>38</v>
+      </c>
       <c r="F72" t="s">
         <v>1</v>
       </c>
@@ -1942,8 +3707,38 @@
       <c r="D73">
         <v>475</v>
       </c>
+      <c r="E73">
+        <v>177</v>
+      </c>
       <c r="F73">
         <v>0.99837900000000002</v>
+      </c>
+      <c r="G73">
+        <v>0.99837900000000002</v>
+      </c>
+      <c r="H73">
+        <v>0.96717900000000001</v>
+      </c>
+      <c r="I73">
+        <v>0.53320500000000004</v>
+      </c>
+      <c r="J73">
+        <v>0.27845900000000001</v>
+      </c>
+      <c r="K73">
+        <v>0.14118900000000001</v>
+      </c>
+      <c r="O73" s="3">
+        <f>I73/F73</f>
+        <v>0.53407072865114358</v>
+      </c>
+      <c r="P73" s="3">
+        <f t="shared" ref="P73:Q73" si="12">J73/G73</f>
+        <v>0.27891111491728093</v>
+      </c>
+      <c r="Q73" s="3">
+        <f t="shared" si="12"/>
+        <v>0.14598021669204977</v>
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.2">
@@ -1959,8 +3754,38 @@
       <c r="D74">
         <v>433</v>
       </c>
+      <c r="E74">
+        <v>154</v>
+      </c>
       <c r="F74">
         <v>0.96645099999999995</v>
+      </c>
+      <c r="G74">
+        <v>0.96645099999999995</v>
+      </c>
+      <c r="H74">
+        <v>0.96645099999999995</v>
+      </c>
+      <c r="I74">
+        <v>0.39710899999999999</v>
+      </c>
+      <c r="J74">
+        <v>0.198576</v>
+      </c>
+      <c r="K74">
+        <v>9.9290000000000003E-2</v>
+      </c>
+      <c r="O74" s="3">
+        <f t="shared" ref="O74:O86" si="13">I74/F74</f>
+        <v>0.41089408568049496</v>
+      </c>
+      <c r="P74" s="3">
+        <f t="shared" ref="P74:P86" si="14">J74/G74</f>
+        <v>0.20546928918279356</v>
+      </c>
+      <c r="Q74" s="3">
+        <f t="shared" ref="Q74:Q86" si="15">K74/H74</f>
+        <v>0.10273671401861037</v>
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.2">
@@ -1976,8 +3801,38 @@
       <c r="D75">
         <v>421</v>
       </c>
+      <c r="E75">
+        <v>118</v>
+      </c>
       <c r="F75">
         <v>0.99997999999999998</v>
+      </c>
+      <c r="G75">
+        <v>0.99997999999999998</v>
+      </c>
+      <c r="H75">
+        <v>0.97136</v>
+      </c>
+      <c r="I75">
+        <v>0.29846299999999998</v>
+      </c>
+      <c r="J75">
+        <v>0.149308</v>
+      </c>
+      <c r="K75">
+        <v>7.4665999999999996E-2</v>
+      </c>
+      <c r="O75" s="3">
+        <f t="shared" si="13"/>
+        <v>0.29846896937938755</v>
+      </c>
+      <c r="P75" s="3">
+        <f t="shared" si="14"/>
+        <v>0.14931098621972438</v>
+      </c>
+      <c r="Q75" s="3">
+        <f t="shared" si="15"/>
+        <v>7.6867484763630367E-2</v>
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.2">
@@ -1993,8 +3848,38 @@
       <c r="D76">
         <v>1471</v>
       </c>
+      <c r="E76">
+        <v>440</v>
+      </c>
       <c r="F76">
         <v>0.97819599999999995</v>
+      </c>
+      <c r="G76">
+        <v>0.97819599999999995</v>
+      </c>
+      <c r="H76">
+        <v>0.97819599999999995</v>
+      </c>
+      <c r="I76">
+        <v>0.13636200000000001</v>
+      </c>
+      <c r="J76">
+        <v>6.8252999999999994E-2</v>
+      </c>
+      <c r="K76">
+        <v>3.4143E-2</v>
+      </c>
+      <c r="O76" s="3">
+        <f t="shared" si="13"/>
+        <v>0.13940151053572086</v>
+      </c>
+      <c r="P76" s="3">
+        <f t="shared" si="14"/>
+        <v>6.9774360148681852E-2</v>
+      </c>
+      <c r="Q76" s="3">
+        <f t="shared" si="15"/>
+        <v>3.4904047859529178E-2</v>
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.2">
@@ -2010,8 +3895,38 @@
       <c r="D77">
         <v>197</v>
       </c>
+      <c r="E77">
+        <v>117</v>
+      </c>
       <c r="F77">
         <v>0.98170100000000005</v>
+      </c>
+      <c r="G77">
+        <v>0.98170100000000005</v>
+      </c>
+      <c r="H77">
+        <v>0.97786799999999996</v>
+      </c>
+      <c r="I77">
+        <v>4.8313000000000002E-2</v>
+      </c>
+      <c r="J77">
+        <v>2.4187E-2</v>
+      </c>
+      <c r="K77">
+        <v>3.4063000000000003E-2</v>
+      </c>
+      <c r="O77" s="3">
+        <f t="shared" si="13"/>
+        <v>4.9213558914577862E-2</v>
+      </c>
+      <c r="P77" s="3">
+        <f t="shared" si="14"/>
+        <v>2.4637847980189486E-2</v>
+      </c>
+      <c r="Q77" s="3">
+        <f t="shared" si="15"/>
+        <v>3.4833944867814472E-2</v>
       </c>
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.2">
@@ -2027,8 +3942,38 @@
       <c r="D78">
         <v>2542</v>
       </c>
+      <c r="E78">
+        <v>235</v>
+      </c>
       <c r="F78">
         <v>0.99998100000000001</v>
+      </c>
+      <c r="G78">
+        <v>0.99998699999999996</v>
+      </c>
+      <c r="H78">
+        <v>0.95849099999999998</v>
+      </c>
+      <c r="I78">
+        <v>0.48976700000000001</v>
+      </c>
+      <c r="J78">
+        <v>0.258351</v>
+      </c>
+      <c r="K78">
+        <v>0.12946199999999999</v>
+      </c>
+      <c r="O78" s="3">
+        <f t="shared" si="13"/>
+        <v>0.48977630574980924</v>
+      </c>
+      <c r="P78" s="3">
+        <f t="shared" si="14"/>
+        <v>0.25835435860666189</v>
+      </c>
+      <c r="Q78" s="3">
+        <f t="shared" si="15"/>
+        <v>0.1350685608941555</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.2">
@@ -2044,8 +3989,38 @@
       <c r="D79">
         <v>89</v>
       </c>
+      <c r="E79">
+        <v>68</v>
+      </c>
       <c r="F79">
         <v>0.96916400000000003</v>
+      </c>
+      <c r="G79">
+        <v>0.96497599999999994</v>
+      </c>
+      <c r="H79">
+        <v>0.96497599999999994</v>
+      </c>
+      <c r="I79">
+        <v>0.35833199999999998</v>
+      </c>
+      <c r="J79">
+        <v>0.422736</v>
+      </c>
+      <c r="K79">
+        <v>0.27588600000000002</v>
+      </c>
+      <c r="O79" s="3">
+        <f t="shared" si="13"/>
+        <v>0.36973308954934353</v>
+      </c>
+      <c r="P79" s="3">
+        <f t="shared" si="14"/>
+        <v>0.438079289018587</v>
+      </c>
+      <c r="Q79" s="3">
+        <f t="shared" si="15"/>
+        <v>0.28589933842914234</v>
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.2">
@@ -2061,6 +4036,39 @@
       <c r="D80">
         <v>909</v>
       </c>
+      <c r="E80">
+        <v>189</v>
+      </c>
+      <c r="F80">
+        <v>0.99384600000000001</v>
+      </c>
+      <c r="G80">
+        <v>0.99384600000000001</v>
+      </c>
+      <c r="H80">
+        <v>0.96278900000000001</v>
+      </c>
+      <c r="I80">
+        <v>0.29606700000000002</v>
+      </c>
+      <c r="J80">
+        <v>0.14808099999999999</v>
+      </c>
+      <c r="K80">
+        <v>7.4052000000000007E-2</v>
+      </c>
+      <c r="O80" s="3">
+        <f t="shared" si="13"/>
+        <v>0.29790027831273658</v>
+      </c>
+      <c r="P80" s="3">
+        <f t="shared" si="14"/>
+        <v>0.14899793328141381</v>
+      </c>
+      <c r="Q80" s="3">
+        <f t="shared" si="15"/>
+        <v>7.6914048664868423E-2</v>
+      </c>
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
@@ -2075,6 +4083,39 @@
       <c r="D81">
         <v>747</v>
       </c>
+      <c r="E81">
+        <v>190</v>
+      </c>
+      <c r="F81">
+        <v>0.99998299999999996</v>
+      </c>
+      <c r="G81">
+        <v>0.97610699999999995</v>
+      </c>
+      <c r="H81">
+        <v>0.97610699999999995</v>
+      </c>
+      <c r="I81">
+        <v>0.33397300000000002</v>
+      </c>
+      <c r="J81">
+        <v>0.167046</v>
+      </c>
+      <c r="K81">
+        <v>8.3537E-2</v>
+      </c>
+      <c r="O81" s="3">
+        <f t="shared" si="13"/>
+        <v>0.33397867763751987</v>
+      </c>
+      <c r="P81" s="3">
+        <f t="shared" si="14"/>
+        <v>0.17113492680618006</v>
+      </c>
+      <c r="Q81" s="3">
+        <f t="shared" si="15"/>
+        <v>8.5581806092979565E-2</v>
+      </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
@@ -2089,6 +4130,39 @@
       <c r="D82">
         <v>855</v>
       </c>
+      <c r="E82">
+        <v>200</v>
+      </c>
+      <c r="F82">
+        <v>0.98175000000000001</v>
+      </c>
+      <c r="G82">
+        <v>0.98175000000000001</v>
+      </c>
+      <c r="H82">
+        <v>0.98175000000000001</v>
+      </c>
+      <c r="I82">
+        <v>0.31838499999999997</v>
+      </c>
+      <c r="J82">
+        <v>0.15924099999999999</v>
+      </c>
+      <c r="K82">
+        <v>7.9631999999999994E-2</v>
+      </c>
+      <c r="O82" s="3">
+        <f t="shared" si="13"/>
+        <v>0.32430353959765723</v>
+      </c>
+      <c r="P82" s="3">
+        <f t="shared" si="14"/>
+        <v>0.16220117137764195</v>
+      </c>
+      <c r="Q82" s="3">
+        <f t="shared" si="15"/>
+        <v>8.1112299465240636E-2</v>
+      </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
@@ -2103,6 +4177,39 @@
       <c r="D83">
         <v>1017</v>
       </c>
+      <c r="E83">
+        <v>215</v>
+      </c>
+      <c r="F83">
+        <v>0.99999300000000002</v>
+      </c>
+      <c r="G83">
+        <v>0.95106299999999999</v>
+      </c>
+      <c r="H83">
+        <v>0.95106299999999999</v>
+      </c>
+      <c r="I83">
+        <v>0.31779600000000002</v>
+      </c>
+      <c r="J83">
+        <v>0.15895100000000001</v>
+      </c>
+      <c r="K83">
+        <v>7.9488000000000003E-2</v>
+      </c>
+      <c r="O83" s="3">
+        <f t="shared" si="13"/>
+        <v>0.31779822458757212</v>
+      </c>
+      <c r="P83" s="3">
+        <f t="shared" si="14"/>
+        <v>0.16712983261886963</v>
+      </c>
+      <c r="Q83" s="3">
+        <f t="shared" si="15"/>
+        <v>8.3578059497635804E-2</v>
+      </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
@@ -2117,6 +4224,39 @@
       <c r="D84">
         <v>1017</v>
       </c>
+      <c r="E84">
+        <v>215</v>
+      </c>
+      <c r="F84">
+        <v>0.99998399999999998</v>
+      </c>
+      <c r="G84">
+        <v>0.95915799999999996</v>
+      </c>
+      <c r="H84">
+        <v>0.95915799999999996</v>
+      </c>
+      <c r="I84">
+        <v>0.335202</v>
+      </c>
+      <c r="J84">
+        <v>0.16764999999999999</v>
+      </c>
+      <c r="K84">
+        <v>8.3836999999999995E-2</v>
+      </c>
+      <c r="O84" s="3">
+        <f t="shared" si="13"/>
+        <v>0.33520736331781309</v>
+      </c>
+      <c r="P84" s="3">
+        <f t="shared" si="14"/>
+        <v>0.17478872094065837</v>
+      </c>
+      <c r="Q84" s="3">
+        <f t="shared" si="15"/>
+        <v>8.7406871443495238E-2</v>
+      </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
@@ -2131,6 +4271,39 @@
       <c r="D85">
         <v>963</v>
       </c>
+      <c r="E85">
+        <v>230</v>
+      </c>
+      <c r="F85">
+        <v>0.99999800000000005</v>
+      </c>
+      <c r="G85">
+        <v>0.99999099999999996</v>
+      </c>
+      <c r="H85">
+        <v>0.96967300000000001</v>
+      </c>
+      <c r="I85">
+        <v>0.33829399999999998</v>
+      </c>
+      <c r="J85">
+        <v>0.16919100000000001</v>
+      </c>
+      <c r="K85">
+        <v>8.4606000000000001E-2</v>
+      </c>
+      <c r="O85" s="3">
+        <f t="shared" si="13"/>
+        <v>0.33829467658935314</v>
+      </c>
+      <c r="P85" s="3">
+        <f t="shared" si="14"/>
+        <v>0.1691925227327046</v>
+      </c>
+      <c r="Q85" s="3">
+        <f t="shared" si="15"/>
+        <v>8.7252094262705054E-2</v>
+      </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
@@ -2144,6 +4317,39 @@
       </c>
       <c r="D86">
         <v>1179</v>
+      </c>
+      <c r="E86">
+        <v>192</v>
+      </c>
+      <c r="F86">
+        <v>0.99998100000000001</v>
+      </c>
+      <c r="G86">
+        <v>0.99997800000000003</v>
+      </c>
+      <c r="H86">
+        <v>0.97653400000000001</v>
+      </c>
+      <c r="I86">
+        <v>0.35473700000000002</v>
+      </c>
+      <c r="J86">
+        <v>0.17741499999999999</v>
+      </c>
+      <c r="K86">
+        <v>8.8719000000000006E-2</v>
+      </c>
+      <c r="O86" s="3">
+        <f t="shared" si="13"/>
+        <v>0.35474374013106252</v>
+      </c>
+      <c r="P86" s="3">
+        <f t="shared" si="14"/>
+        <v>0.17741890321587073</v>
+      </c>
+      <c r="Q86" s="3">
+        <f t="shared" si="15"/>
+        <v>9.0850907392881361E-2</v>
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.2">
@@ -2189,6 +4395,9 @@
       <c r="D89" t="s">
         <v>25</v>
       </c>
+      <c r="E89" t="s">
+        <v>38</v>
+      </c>
       <c r="F89" t="s">
         <v>1</v>
       </c>
@@ -2248,8 +4457,38 @@
       <c r="D90">
         <v>475</v>
       </c>
+      <c r="E90">
+        <v>177</v>
+      </c>
       <c r="F90">
-        <v>0.90542199999999995</v>
+        <v>0.89998100000000003</v>
+      </c>
+      <c r="G90">
+        <v>0.81923800000000002</v>
+      </c>
+      <c r="H90">
+        <v>0.64998599999999995</v>
+      </c>
+      <c r="I90">
+        <v>0.53320500000000004</v>
+      </c>
+      <c r="J90">
+        <v>0.27845900000000001</v>
+      </c>
+      <c r="K90">
+        <v>0.13933100000000001</v>
+      </c>
+      <c r="O90" s="3">
+        <f>I90/F90</f>
+        <v>0.59246250754182594</v>
+      </c>
+      <c r="P90" s="3">
+        <f t="shared" ref="P90:Q90" si="16">J90/G90</f>
+        <v>0.33990000463845671</v>
+      </c>
+      <c r="Q90" s="3">
+        <f t="shared" si="16"/>
+        <v>0.21436000160003449</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.2">
@@ -2265,8 +4504,38 @@
       <c r="D91">
         <v>433</v>
       </c>
+      <c r="E91">
+        <v>154</v>
+      </c>
       <c r="F91">
-        <v>0.84776399999999996</v>
+        <v>0.85526599999999997</v>
+      </c>
+      <c r="G91">
+        <v>0.76702499999999996</v>
+      </c>
+      <c r="H91">
+        <v>0.63582300000000003</v>
+      </c>
+      <c r="I91">
+        <v>0.39710899999999999</v>
+      </c>
+      <c r="J91">
+        <v>0.198576</v>
+      </c>
+      <c r="K91">
+        <v>9.8632999999999998E-2</v>
+      </c>
+      <c r="O91" s="3">
+        <f t="shared" ref="O91:O103" si="17">I91/F91</f>
+        <v>0.46431051859889205</v>
+      </c>
+      <c r="P91" s="3">
+        <f t="shared" ref="P91:P103" si="18">J91/G91</f>
+        <v>0.25889117043121151</v>
+      </c>
+      <c r="Q91" s="3">
+        <f t="shared" ref="Q91:Q103" si="19">K91/H91</f>
+        <v>0.15512650533245886</v>
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.2">
@@ -2282,8 +4551,38 @@
       <c r="D92">
         <v>421</v>
       </c>
+      <c r="E92">
+        <v>118</v>
+      </c>
       <c r="F92">
-        <v>0.90948600000000002</v>
+        <v>0.91699200000000003</v>
+      </c>
+      <c r="G92">
+        <v>0.84232499999999999</v>
+      </c>
+      <c r="H92">
+        <v>0.70928100000000005</v>
+      </c>
+      <c r="I92">
+        <v>0.296095</v>
+      </c>
+      <c r="J92">
+        <v>0.148123</v>
+      </c>
+      <c r="K92">
+        <v>7.4073E-2</v>
+      </c>
+      <c r="O92" s="3">
+        <f t="shared" si="17"/>
+        <v>0.32289812779173643</v>
+      </c>
+      <c r="P92" s="3">
+        <f t="shared" si="18"/>
+        <v>0.17585017659454485</v>
+      </c>
+      <c r="Q92" s="3">
+        <f t="shared" si="19"/>
+        <v>0.10443392675117477</v>
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.2">
@@ -2299,8 +4598,38 @@
       <c r="D93">
         <v>1471</v>
       </c>
+      <c r="E93">
+        <v>440</v>
+      </c>
       <c r="F93">
-        <v>0.86413099999999998</v>
+        <v>0.86209999999999998</v>
+      </c>
+      <c r="G93">
+        <v>0.77063800000000005</v>
+      </c>
+      <c r="H93">
+        <v>0.63574299999999995</v>
+      </c>
+      <c r="I93">
+        <v>0.13636200000000001</v>
+      </c>
+      <c r="J93">
+        <v>6.8252999999999994E-2</v>
+      </c>
+      <c r="K93">
+        <v>3.4143E-2</v>
+      </c>
+      <c r="O93" s="3">
+        <f t="shared" si="17"/>
+        <v>0.15817422572787382</v>
+      </c>
+      <c r="P93" s="3">
+        <f t="shared" si="18"/>
+        <v>8.8566875757489241E-2</v>
+      </c>
+      <c r="Q93" s="3">
+        <f t="shared" si="19"/>
+        <v>5.3705664081240383E-2</v>
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.2">
@@ -2316,8 +4645,38 @@
       <c r="D94">
         <v>197</v>
       </c>
+      <c r="E94">
+        <v>117</v>
+      </c>
       <c r="F94">
-        <v>0.91165499999999999</v>
+        <v>0.91264400000000001</v>
+      </c>
+      <c r="G94">
+        <v>0.853406</v>
+      </c>
+      <c r="H94">
+        <v>0.73812100000000003</v>
+      </c>
+      <c r="I94">
+        <v>4.8313000000000002E-2</v>
+      </c>
+      <c r="J94">
+        <v>2.4187E-2</v>
+      </c>
+      <c r="K94">
+        <v>2.4160000000000001E-2</v>
+      </c>
+      <c r="O94" s="3">
+        <f t="shared" si="17"/>
+        <v>5.2937399467919581E-2</v>
+      </c>
+      <c r="P94" s="3">
+        <f t="shared" si="18"/>
+        <v>2.8341727149797401E-2</v>
+      </c>
+      <c r="Q94" s="3">
+        <f t="shared" si="19"/>
+        <v>3.2731760781768843E-2</v>
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.2">
@@ -2333,8 +4692,38 @@
       <c r="D95">
         <v>2542</v>
       </c>
+      <c r="E95">
+        <v>235</v>
+      </c>
       <c r="F95">
-        <v>0.90701299999999996</v>
+        <v>0.90359800000000001</v>
+      </c>
+      <c r="G95">
+        <v>0.83962000000000003</v>
+      </c>
+      <c r="H95">
+        <v>0.70039499999999999</v>
+      </c>
+      <c r="I95">
+        <v>0.48976700000000001</v>
+      </c>
+      <c r="J95">
+        <v>0.25663999999999998</v>
+      </c>
+      <c r="K95">
+        <v>0.128605</v>
+      </c>
+      <c r="O95" s="3">
+        <f t="shared" si="17"/>
+        <v>0.5420186853003216</v>
+      </c>
+      <c r="P95" s="3">
+        <f t="shared" si="18"/>
+        <v>0.30566208522903215</v>
+      </c>
+      <c r="Q95" s="3">
+        <f t="shared" si="19"/>
+        <v>0.18361781566116261</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.2">
@@ -2350,11 +4739,41 @@
       <c r="D96">
         <v>89</v>
       </c>
+      <c r="E96">
+        <v>68</v>
+      </c>
       <c r="F96">
         <v>0.88306499999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G96">
+        <v>0.81101599999999996</v>
+      </c>
+      <c r="H96">
+        <v>0.69723999999999997</v>
+      </c>
+      <c r="I96">
+        <v>0.35726000000000002</v>
+      </c>
+      <c r="J96">
+        <v>0.35137000000000002</v>
+      </c>
+      <c r="K96">
+        <v>0.25918799999999997</v>
+      </c>
+      <c r="O96" s="3">
+        <f t="shared" si="17"/>
+        <v>0.40456818014528945</v>
+      </c>
+      <c r="P96" s="3">
+        <f t="shared" si="18"/>
+        <v>0.43324669303688218</v>
+      </c>
+      <c r="Q96" s="3">
+        <f t="shared" si="19"/>
+        <v>0.37173426653663011</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -2367,8 +4786,41 @@
       <c r="D97">
         <v>909</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E97">
+        <v>189</v>
+      </c>
+      <c r="F97">
+        <v>0.89054299999999997</v>
+      </c>
+      <c r="G97">
+        <v>0.80669400000000002</v>
+      </c>
+      <c r="H97">
+        <v>0.63599399999999995</v>
+      </c>
+      <c r="I97">
+        <v>0.29217100000000001</v>
+      </c>
+      <c r="J97">
+        <v>0.14613200000000001</v>
+      </c>
+      <c r="K97">
+        <v>7.3078000000000004E-2</v>
+      </c>
+      <c r="O97" s="3">
+        <f t="shared" si="17"/>
+        <v>0.32808185567681741</v>
+      </c>
+      <c r="P97" s="3">
+        <f t="shared" si="18"/>
+        <v>0.18114923378629319</v>
+      </c>
+      <c r="Q97" s="3">
+        <f t="shared" si="19"/>
+        <v>0.11490359971949422</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>12</v>
       </c>
@@ -2381,8 +4833,41 @@
       <c r="D98">
         <v>747</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E98">
+        <v>190</v>
+      </c>
+      <c r="F98">
+        <v>0.86917299999999997</v>
+      </c>
+      <c r="G98">
+        <v>0.76727900000000004</v>
+      </c>
+      <c r="H98">
+        <v>0.63096799999999997</v>
+      </c>
+      <c r="I98">
+        <v>0.32957900000000001</v>
+      </c>
+      <c r="J98">
+        <v>0.16594</v>
+      </c>
+      <c r="K98">
+        <v>8.2436999999999996E-2</v>
+      </c>
+      <c r="O98" s="3">
+        <f t="shared" si="17"/>
+        <v>0.37918688224323582</v>
+      </c>
+      <c r="P98" s="3">
+        <f t="shared" si="18"/>
+        <v>0.21627074375813751</v>
+      </c>
+      <c r="Q98" s="3">
+        <f t="shared" si="19"/>
+        <v>0.13065163368031343</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>13</v>
       </c>
@@ -2395,8 +4880,41 @@
       <c r="D99">
         <v>855</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E99">
+        <v>200</v>
+      </c>
+      <c r="F99">
+        <v>0.87656299999999998</v>
+      </c>
+      <c r="G99">
+        <v>0.79237299999999999</v>
+      </c>
+      <c r="H99">
+        <v>0.66364400000000001</v>
+      </c>
+      <c r="I99">
+        <v>0.31419599999999998</v>
+      </c>
+      <c r="J99">
+        <v>0.15818599999999999</v>
+      </c>
+      <c r="K99">
+        <v>7.8584000000000001E-2</v>
+      </c>
+      <c r="O99" s="3">
+        <f t="shared" si="17"/>
+        <v>0.35844086506046913</v>
+      </c>
+      <c r="P99" s="3">
+        <f t="shared" si="18"/>
+        <v>0.19963577759464293</v>
+      </c>
+      <c r="Q99" s="3">
+        <f t="shared" si="19"/>
+        <v>0.11841288401612914</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>14</v>
       </c>
@@ -2409,8 +4927,41 @@
       <c r="D100">
         <v>1017</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E100">
+        <v>215</v>
+      </c>
+      <c r="F100">
+        <v>0.88547200000000004</v>
+      </c>
+      <c r="G100">
+        <v>0.76739900000000005</v>
+      </c>
+      <c r="H100">
+        <v>0.643625</v>
+      </c>
+      <c r="I100">
+        <v>0.31361499999999998</v>
+      </c>
+      <c r="J100">
+        <v>0.15789800000000001</v>
+      </c>
+      <c r="K100">
+        <v>7.8441999999999998E-2</v>
+      </c>
+      <c r="O100" s="3">
+        <f t="shared" si="17"/>
+        <v>0.35417833652560438</v>
+      </c>
+      <c r="P100" s="3">
+        <f t="shared" si="18"/>
+        <v>0.20575737002524111</v>
+      </c>
+      <c r="Q100" s="3">
+        <f t="shared" si="19"/>
+        <v>0.12187531559526121</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>15</v>
       </c>
@@ -2423,8 +4974,41 @@
       <c r="D101">
         <v>1017</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E101">
+        <v>215</v>
+      </c>
+      <c r="F101">
+        <v>0.90088599999999996</v>
+      </c>
+      <c r="G101">
+        <v>0.79389600000000005</v>
+      </c>
+      <c r="H101">
+        <v>0.67769100000000004</v>
+      </c>
+      <c r="I101">
+        <v>0.33079199999999997</v>
+      </c>
+      <c r="J101">
+        <v>0.16653999999999999</v>
+      </c>
+      <c r="K101">
+        <v>8.2734000000000002E-2</v>
+      </c>
+      <c r="O101" s="3">
+        <f t="shared" si="17"/>
+        <v>0.36718519324309623</v>
+      </c>
+      <c r="P101" s="3">
+        <f t="shared" si="18"/>
+        <v>0.20977558773441354</v>
+      </c>
+      <c r="Q101" s="3">
+        <f t="shared" si="19"/>
+        <v>0.12208218789979504</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -2437,8 +5021,41 @@
       <c r="D102">
         <v>963</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E102">
+        <v>230</v>
+      </c>
+      <c r="F102">
+        <v>0.91491100000000003</v>
+      </c>
+      <c r="G102">
+        <v>0.850935</v>
+      </c>
+      <c r="H102">
+        <v>0.71404500000000004</v>
+      </c>
+      <c r="I102">
+        <v>0.333843</v>
+      </c>
+      <c r="J102">
+        <v>0.166964</v>
+      </c>
+      <c r="K102">
+        <v>8.3492999999999998E-2</v>
+      </c>
+      <c r="O102" s="3">
+        <f t="shared" si="17"/>
+        <v>0.36489122985733036</v>
+      </c>
+      <c r="P102" s="3">
+        <f t="shared" si="18"/>
+        <v>0.19621240165230011</v>
+      </c>
+      <c r="Q102" s="3">
+        <f t="shared" si="19"/>
+        <v>0.11692960527697834</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>17</v>
       </c>
@@ -2451,19 +5068,50 @@
       <c r="D103">
         <v>1179</v>
       </c>
+      <c r="E103">
+        <v>192</v>
+      </c>
+      <c r="F103">
+        <v>0.907698</v>
+      </c>
+      <c r="G103">
+        <v>0.84815799999999997</v>
+      </c>
+      <c r="H103">
+        <v>0.72866600000000004</v>
+      </c>
+      <c r="I103">
+        <v>0.35006900000000002</v>
+      </c>
+      <c r="J103">
+        <v>0.17624100000000001</v>
+      </c>
+      <c r="K103">
+        <v>8.7552000000000005E-2</v>
+      </c>
+      <c r="O103" s="3">
+        <f t="shared" si="17"/>
+        <v>0.38566681869961156</v>
+      </c>
+      <c r="P103" s="3">
+        <f t="shared" si="18"/>
+        <v>0.20779265184081269</v>
+      </c>
+      <c r="Q103" s="3">
+        <f t="shared" si="19"/>
+        <v>0.12015381532828484</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="F88:H88"/>
-    <mergeCell ref="I88:K88"/>
-    <mergeCell ref="L88:N88"/>
-    <mergeCell ref="O88:Q88"/>
-    <mergeCell ref="R88:T88"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="R20:T20"/>
-    <mergeCell ref="R37:T37"/>
-    <mergeCell ref="R54:T54"/>
-    <mergeCell ref="R71:T71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="I71:K71"/>
+    <mergeCell ref="O71:Q71"/>
+    <mergeCell ref="F54:H54"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="O54:Q54"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="L71:N71"/>
     <mergeCell ref="L3:N3"/>
     <mergeCell ref="L20:N20"/>
     <mergeCell ref="F37:H37"/>
@@ -2476,14 +5124,16 @@
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="I20:K20"/>
     <mergeCell ref="O20:Q20"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="I71:K71"/>
-    <mergeCell ref="O71:Q71"/>
-    <mergeCell ref="F54:H54"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="O54:Q54"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="L71:N71"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="R20:T20"/>
+    <mergeCell ref="R37:T37"/>
+    <mergeCell ref="R54:T54"/>
+    <mergeCell ref="R71:T71"/>
+    <mergeCell ref="F88:H88"/>
+    <mergeCell ref="I88:K88"/>
+    <mergeCell ref="L88:N88"/>
+    <mergeCell ref="O88:Q88"/>
+    <mergeCell ref="R88:T88"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update result and readme
</commit_message>
<xml_diff>
--- a/result/result.xlsx
+++ b/result/result.xlsx
@@ -2658,7 +2658,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="179" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -2709,11 +2709,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
@@ -2992,10 +2992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W120"/>
+  <dimension ref="A1:X120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" zoomScale="117" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107:C120"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="117" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3007,9 +3007,10 @@
     <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="12" max="12" width="14.6640625" customWidth="1"/>
     <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="24" max="24" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3029,7 +3030,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -3049,42 +3050,42 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2" t="s">
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2" t="s">
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -3155,7 +3156,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>60</v>
       </c>
       <c r="P5" s="1">
-        <f t="shared" ref="P5:W5" si="0">(H5-D5)/H5</f>
+        <f t="shared" ref="P5:R5" si="0">(H5-D5)/H5</f>
         <v>0.39557351536663338</v>
       </c>
       <c r="Q5" s="1">
@@ -3233,8 +3234,9 @@
         <f t="shared" si="1"/>
         <v>0.79514314877832903</v>
       </c>
+      <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3285,7 +3287,7 @@
         <v>0.42071651227560442</v>
       </c>
       <c r="Q6" s="1">
-        <f t="shared" ref="Q6:W18" si="2">(I6-E6)/I6</f>
+        <f t="shared" ref="Q6:S18" si="2">(I6-E6)/I6</f>
         <v>0.59059703745781233</v>
       </c>
       <c r="R6" s="1">
@@ -3312,8 +3314,9 @@
         <f t="shared" si="1"/>
         <v>0.867423405450792</v>
       </c>
+      <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>214</v>
       </c>
@@ -3391,8 +3394,9 @@
         <f t="shared" si="1"/>
         <v>0.92290291335205288</v>
       </c>
+      <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3470,8 +3474,9 @@
         <f t="shared" si="1"/>
         <v>0.91685498380492947</v>
       </c>
+      <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -3549,8 +3554,9 @@
         <f t="shared" si="1"/>
         <v>0.96287252217392849</v>
       </c>
+      <c r="X9" s="3"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>215</v>
       </c>
@@ -3628,8 +3634,9 @@
         <f t="shared" si="1"/>
         <v>0.94045925713266609</v>
       </c>
+      <c r="X10" s="3"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -3707,8 +3714,9 @@
         <f t="shared" si="1"/>
         <v>0.96531026240337747</v>
       </c>
+      <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -3786,8 +3794,9 @@
         <f t="shared" si="1"/>
         <v>0.97800433481779359</v>
       </c>
+      <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -3865,8 +3874,9 @@
         <f t="shared" si="1"/>
         <v>0.97503510305873309</v>
       </c>
+      <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -3944,8 +3954,9 @@
         <f t="shared" si="1"/>
         <v>0.97959215962875157</v>
       </c>
+      <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -4023,8 +4034,9 @@
         <f t="shared" si="1"/>
         <v>0.98032887805802471</v>
       </c>
+      <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -4102,8 +4114,9 @@
         <f t="shared" si="1"/>
         <v>0.98005478503182453</v>
       </c>
+      <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>216</v>
       </c>
@@ -4150,7 +4163,7 @@
         <v>204</v>
       </c>
       <c r="P17" s="1">
-        <f t="shared" ref="P17:W17" si="5">(H17-D17)/H17</f>
+        <f t="shared" ref="P17:S17" si="5">(H17-D17)/H17</f>
         <v>0.46561987617726369</v>
       </c>
       <c r="Q17" s="1">
@@ -4181,8 +4194,9 @@
         <f t="shared" si="1"/>
         <v>0.97906418267073392</v>
       </c>
+      <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -4260,46 +4274,47 @@
         <f t="shared" si="1"/>
         <v>0.9798595928349173</v>
       </c>
+      <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="Q19" s="1"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>217</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2" t="s">
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2" t="s">
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2" t="s">
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
-      <c r="W20" s="2"/>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="4"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -4370,7 +4385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -4416,40 +4431,40 @@
       <c r="O22" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="4">
+      <c r="P22" s="3">
         <f>H22/D22</f>
         <v>1.0918781602193115</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="Q22" s="3">
         <f t="shared" ref="Q22:S35" si="6">I22/E22</f>
         <v>2.1587600782778864</v>
       </c>
-      <c r="R22" s="4">
+      <c r="R22" s="3">
         <f t="shared" si="6"/>
         <v>5.1153682888540031</v>
       </c>
-      <c r="S22" s="4">
+      <c r="S22" s="3">
         <f t="shared" si="6"/>
         <v>5.1727931034482761</v>
       </c>
-      <c r="T22" s="4">
+      <c r="T22" s="3">
         <f>L22/D22</f>
         <v>3.76060706670728</v>
       </c>
-      <c r="U22" s="4">
+      <c r="U22" s="3">
         <f t="shared" ref="U22:W35" si="7">M22/E22</f>
         <v>4.5923034572733199</v>
       </c>
-      <c r="V22" s="4">
+      <c r="V22" s="3">
         <f t="shared" si="7"/>
         <v>7.4586854003139713</v>
       </c>
-      <c r="W22" s="4">
+      <c r="W22" s="3">
         <f t="shared" si="7"/>
         <v>16.327633497536947</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -4495,40 +4510,40 @@
       <c r="O23" t="s">
         <v>72</v>
       </c>
-      <c r="P23" s="4">
+      <c r="P23" s="3">
         <f t="shared" ref="P23:P35" si="8">H23/D23</f>
         <v>0.82554848260547742</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="Q23" s="3">
         <f t="shared" si="6"/>
         <v>1.1739731694828468</v>
       </c>
-      <c r="R23" s="4">
+      <c r="R23" s="3">
         <f t="shared" si="6"/>
         <v>2.2932329411764707</v>
       </c>
-      <c r="S23" s="4">
+      <c r="S23" s="3">
         <f t="shared" si="6"/>
         <v>4.9349920634920634</v>
       </c>
-      <c r="T23" s="4">
+      <c r="T23" s="3">
         <f t="shared" ref="T23:T35" si="9">L23/D23</f>
         <v>3.3807905255366397</v>
       </c>
-      <c r="U23" s="4">
+      <c r="U23" s="3">
         <f t="shared" si="7"/>
         <v>4.9320928315412189</v>
       </c>
-      <c r="V23" s="4">
+      <c r="V23" s="3">
         <f t="shared" si="7"/>
         <v>7.36854431372549</v>
       </c>
-      <c r="W23" s="4">
+      <c r="W23" s="3">
         <f t="shared" si="7"/>
         <v>13.828484126984128</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>214</v>
       </c>
@@ -4574,40 +4589,40 @@
       <c r="O24" t="s">
         <v>84</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P24" s="3">
         <f t="shared" si="8"/>
         <v>0.92458529239329112</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="Q24" s="3">
         <f t="shared" si="6"/>
         <v>1.4491968076616122</v>
       </c>
-      <c r="R24" s="4">
+      <c r="R24" s="3">
         <f t="shared" si="6"/>
         <v>2.8937351916376306</v>
       </c>
-      <c r="S24" s="4">
+      <c r="S24" s="3">
         <f t="shared" si="6"/>
         <v>31.222952380952382</v>
       </c>
-      <c r="T24" s="4">
+      <c r="T24" s="3">
         <f t="shared" si="9"/>
         <v>6.8935387424463626</v>
       </c>
-      <c r="U24" s="4">
+      <c r="U24" s="3">
         <f t="shared" si="7"/>
         <v>9.7505412609736624</v>
       </c>
-      <c r="V24" s="4">
+      <c r="V24" s="3">
         <f t="shared" si="7"/>
         <v>17.862912543554007</v>
       </c>
-      <c r="W24" s="4">
+      <c r="W24" s="3">
         <f t="shared" si="7"/>
         <v>31.129580952380952</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -4653,40 +4668,40 @@
       <c r="O25" t="s">
         <v>96</v>
       </c>
-      <c r="P25" s="4">
+      <c r="P25" s="3">
         <f t="shared" si="8"/>
         <v>1.24220862467547</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="Q25" s="3">
         <f t="shared" si="6"/>
         <v>1.9592405100235872</v>
       </c>
-      <c r="R25" s="4">
+      <c r="R25" s="3">
         <f t="shared" si="6"/>
         <v>3.1687925482119454</v>
       </c>
-      <c r="S25" s="4">
+      <c r="S25" s="3">
         <f t="shared" si="6"/>
         <v>6.5276734693877554</v>
       </c>
-      <c r="T25" s="4">
+      <c r="T25" s="3">
         <f t="shared" si="9"/>
         <v>6.3943606687641408</v>
       </c>
-      <c r="U25" s="4">
+      <c r="U25" s="3">
         <f t="shared" si="7"/>
         <v>8.4992437474029927</v>
       </c>
-      <c r="V25" s="4">
+      <c r="V25" s="3">
         <f t="shared" si="7"/>
         <v>9.087859576858266</v>
       </c>
-      <c r="W25" s="4">
+      <c r="W25" s="3">
         <f t="shared" si="7"/>
         <v>15.219226617661283</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -4732,40 +4747,40 @@
       <c r="O26" t="s">
         <v>108</v>
       </c>
-      <c r="P26" s="4">
+      <c r="P26" s="3">
         <f t="shared" si="8"/>
         <v>3.1703646793228222</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="Q26" s="3">
         <f t="shared" si="6"/>
         <v>6.3957524561365462</v>
       </c>
-      <c r="R26" s="4">
+      <c r="R26" s="3">
         <f t="shared" si="6"/>
         <v>12.706925643124613</v>
       </c>
-      <c r="S26" s="4">
+      <c r="S26" s="3">
         <f t="shared" si="6"/>
         <v>29.283118817147113</v>
       </c>
-      <c r="T26" s="4">
+      <c r="T26" s="3">
         <f t="shared" si="9"/>
         <v>6.8949882033846883</v>
       </c>
-      <c r="U26" s="4">
+      <c r="U26" s="3">
         <f t="shared" si="7"/>
         <v>11.841340627643193</v>
       </c>
-      <c r="V26" s="4">
+      <c r="V26" s="3">
         <f t="shared" si="7"/>
         <v>19.593031268643948</v>
       </c>
-      <c r="W26" s="4">
+      <c r="W26" s="3">
         <f t="shared" si="7"/>
         <v>42.838250363436515</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>215</v>
       </c>
@@ -4811,40 +4826,40 @@
       <c r="O27" t="s">
         <v>120</v>
       </c>
-      <c r="P27" s="4">
+      <c r="P27" s="3">
         <f t="shared" si="8"/>
         <v>7.9504418704418702</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="Q27" s="3">
         <f t="shared" si="6"/>
         <v>14.368406673014034</v>
       </c>
-      <c r="R27" s="4">
+      <c r="R27" s="3">
         <f t="shared" si="6"/>
         <v>31.359781495390919</v>
       </c>
-      <c r="S27" s="4">
+      <c r="S27" s="3">
         <f t="shared" si="6"/>
         <v>31.199191810344828</v>
       </c>
-      <c r="T27" s="4">
+      <c r="T27" s="3">
         <f t="shared" si="9"/>
         <v>7.1820398970398971</v>
       </c>
-      <c r="U27" s="4">
+      <c r="U27" s="3">
         <f t="shared" si="7"/>
         <v>12.122105393881691</v>
       </c>
-      <c r="V27" s="4">
+      <c r="V27" s="3">
         <f t="shared" si="7"/>
         <v>16.263161488562648</v>
       </c>
-      <c r="W27" s="4">
+      <c r="W27" s="3">
         <f t="shared" si="7"/>
         <v>20.644127155172413</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -4890,40 +4905,40 @@
       <c r="O28" t="s">
         <v>132</v>
       </c>
-      <c r="P28" s="4">
+      <c r="P28" s="3">
         <f t="shared" si="8"/>
         <v>0.29981164779986763</v>
       </c>
-      <c r="Q28" s="4">
+      <c r="Q28" s="3">
         <f t="shared" si="6"/>
         <v>0.18304738503061035</v>
       </c>
-      <c r="R28" s="4">
+      <c r="R28" s="3">
         <f t="shared" si="6"/>
         <v>7.5312848158131177E-2</v>
       </c>
-      <c r="S28" s="4">
+      <c r="S28" s="3">
         <f t="shared" si="6"/>
         <v>4.4028445563247323E-2</v>
       </c>
-      <c r="T28" s="4">
+      <c r="T28" s="3">
         <f t="shared" si="9"/>
         <v>6.6037376157656391</v>
       </c>
-      <c r="U28" s="4">
+      <c r="U28" s="3">
         <f t="shared" si="7"/>
         <v>12.741302537626884</v>
       </c>
-      <c r="V28" s="4">
+      <c r="V28" s="3">
         <f t="shared" si="7"/>
         <v>19.769975172207246</v>
       </c>
-      <c r="W28" s="4">
+      <c r="W28" s="3">
         <f t="shared" si="7"/>
         <v>34.605062240402766</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -4969,40 +4984,40 @@
       <c r="O29" t="s">
         <v>144</v>
       </c>
-      <c r="P29" s="4">
+      <c r="P29" s="3">
         <f t="shared" si="8"/>
         <v>0.46582206295399514</v>
       </c>
-      <c r="Q29" s="4">
+      <c r="Q29" s="3">
         <f t="shared" si="6"/>
         <v>0.55890264039408866</v>
       </c>
-      <c r="R29" s="4">
+      <c r="R29" s="3">
         <f t="shared" si="6"/>
         <v>0.79638857142857145</v>
       </c>
-      <c r="S29" s="4">
+      <c r="S29" s="3">
         <f t="shared" si="6"/>
         <v>1.2410214917825537</v>
       </c>
-      <c r="T29" s="4">
+      <c r="T29" s="3">
         <f t="shared" si="9"/>
         <v>15.121364726392251</v>
       </c>
-      <c r="U29" s="4">
+      <c r="U29" s="3">
         <f t="shared" si="7"/>
         <v>22.109401477832513</v>
       </c>
-      <c r="V29" s="4">
+      <c r="V29" s="3">
         <f t="shared" si="7"/>
         <v>32.301337632653059</v>
       </c>
-      <c r="W29" s="4">
+      <c r="W29" s="3">
         <f t="shared" si="7"/>
         <v>61.55677901390645</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -5048,40 +5063,40 @@
       <c r="O30" t="s">
         <v>156</v>
       </c>
-      <c r="P30" s="4">
+      <c r="P30" s="3">
         <f t="shared" si="8"/>
         <v>0.52182066339606059</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="Q30" s="3">
         <f t="shared" si="6"/>
         <v>0.64153369385609138</v>
       </c>
-      <c r="R30" s="4">
+      <c r="R30" s="3">
         <f t="shared" si="6"/>
         <v>0.93007526132404184</v>
       </c>
-      <c r="S30" s="4">
+      <c r="S30" s="3">
         <f t="shared" si="6"/>
         <v>1.7691019189765458</v>
       </c>
-      <c r="T30" s="4">
+      <c r="T30" s="3">
         <f t="shared" si="9"/>
         <v>13.613894969612653</v>
       </c>
-      <c r="U30" s="4">
+      <c r="U30" s="3">
         <f t="shared" si="7"/>
         <v>18.091665675229081</v>
       </c>
-      <c r="V30" s="4">
+      <c r="V30" s="3">
         <f t="shared" si="7"/>
         <v>29.988262274311055</v>
       </c>
-      <c r="W30" s="4">
+      <c r="W30" s="3">
         <f t="shared" si="7"/>
         <v>59.187584221748402</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -5127,40 +5142,40 @@
       <c r="O31" t="s">
         <v>168</v>
       </c>
-      <c r="P31" s="4">
+      <c r="P31" s="3">
         <f t="shared" si="8"/>
         <v>0.5164199958086384</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="Q31" s="3">
         <f t="shared" si="6"/>
         <v>0.5682161512457744</v>
       </c>
-      <c r="R31" s="4">
+      <c r="R31" s="3">
         <f t="shared" si="6"/>
         <v>0.81319667282809616</v>
       </c>
-      <c r="S31" s="4">
+      <c r="S31" s="3">
         <f t="shared" si="6"/>
         <v>1.4789794569067296</v>
       </c>
-      <c r="T31" s="4">
+      <c r="T31" s="3">
         <f t="shared" si="9"/>
         <v>16.309996116952455</v>
       </c>
-      <c r="U31" s="4">
+      <c r="U31" s="3">
         <f t="shared" si="7"/>
         <v>21.1153497934143</v>
       </c>
-      <c r="V31" s="4">
+      <c r="V31" s="3">
         <f t="shared" si="7"/>
         <v>33.839853076313702</v>
       </c>
-      <c r="W31" s="4">
+      <c r="W31" s="3">
         <f t="shared" si="7"/>
         <v>72.083785123966948</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -5206,35 +5221,35 @@
       <c r="O32" t="s">
         <v>180</v>
       </c>
-      <c r="P32" s="4">
+      <c r="P32" s="3">
         <f t="shared" si="8"/>
         <v>0.40971223087860331</v>
       </c>
-      <c r="Q32" s="4">
+      <c r="Q32" s="3">
         <f t="shared" si="6"/>
         <v>0.44457425542655227</v>
       </c>
-      <c r="R32" s="4">
+      <c r="R32" s="3">
         <f t="shared" si="6"/>
         <v>0.62354285714285718</v>
       </c>
-      <c r="S32" s="4">
+      <c r="S32" s="3">
         <f t="shared" si="6"/>
         <v>1.0720674698795181</v>
       </c>
-      <c r="T32" s="4">
+      <c r="T32" s="3">
         <f t="shared" si="9"/>
         <v>16.744246910622497</v>
       </c>
-      <c r="U32" s="4">
+      <c r="U32" s="3">
         <f t="shared" si="7"/>
         <v>23.867896264512872</v>
       </c>
-      <c r="V32" s="4">
+      <c r="V32" s="3">
         <f t="shared" si="7"/>
         <v>38.264112781954886</v>
       </c>
-      <c r="W32" s="4">
+      <c r="W32" s="3">
         <f t="shared" si="7"/>
         <v>77.785114974182449</v>
       </c>
@@ -5285,35 +5300,35 @@
       <c r="O33" t="s">
         <v>192</v>
       </c>
-      <c r="P33" s="4">
+      <c r="P33" s="3">
         <f t="shared" si="8"/>
         <v>0.35189332039776861</v>
       </c>
-      <c r="Q33" s="4">
+      <c r="Q33" s="3">
         <f t="shared" si="6"/>
         <v>0.40890495304003954</v>
       </c>
-      <c r="R33" s="4">
+      <c r="R33" s="3">
         <f t="shared" si="6"/>
         <v>0.57029788283658789</v>
       </c>
-      <c r="S33" s="4">
+      <c r="S33" s="3">
         <f t="shared" si="6"/>
         <v>0.97783535714285719</v>
       </c>
-      <c r="T33" s="4">
+      <c r="T33" s="3">
         <f t="shared" si="9"/>
         <v>15.214531593499879</v>
       </c>
-      <c r="U33" s="4">
+      <c r="U33" s="3">
         <f t="shared" si="7"/>
         <v>21.988489985170538</v>
       </c>
-      <c r="V33" s="4">
+      <c r="V33" s="3">
         <f t="shared" si="7"/>
         <v>33.288207810894143</v>
       </c>
-      <c r="W33" s="4">
+      <c r="W33" s="3">
         <f t="shared" si="7"/>
         <v>67.058690624999997</v>
       </c>
@@ -5364,35 +5379,35 @@
       <c r="O34" t="s">
         <v>204</v>
       </c>
-      <c r="P34" s="4">
+      <c r="P34" s="3">
         <f t="shared" si="8"/>
         <v>0.30257923757133309</v>
       </c>
-      <c r="Q34" s="4">
+      <c r="Q34" s="3">
         <f t="shared" si="6"/>
         <v>0.29607773087462047</v>
       </c>
-      <c r="R34" s="4">
+      <c r="R34" s="3">
         <f t="shared" si="6"/>
         <v>0.37344642857142857</v>
       </c>
-      <c r="S34" s="4">
+      <c r="S34" s="3">
         <f t="shared" si="6"/>
         <v>0.62600747663551404</v>
       </c>
-      <c r="T34" s="4">
+      <c r="T34" s="3">
         <f t="shared" si="9"/>
         <v>16.643910700285332</v>
       </c>
-      <c r="U34" s="4">
+      <c r="U34" s="3">
         <f t="shared" si="7"/>
         <v>24.303277982670519</v>
       </c>
-      <c r="V34" s="4">
+      <c r="V34" s="3">
         <f t="shared" si="7"/>
         <v>34.306707450738919</v>
       </c>
-      <c r="W34" s="4">
+      <c r="W34" s="3">
         <f t="shared" si="7"/>
         <v>63.61230994659546</v>
       </c>
@@ -5443,35 +5458,35 @@
       <c r="O35" t="s">
         <v>213</v>
       </c>
-      <c r="P35" s="4">
+      <c r="P35" s="3">
         <f t="shared" si="8"/>
         <v>0.40884342857142858</v>
       </c>
-      <c r="Q35" s="4">
+      <c r="Q35" s="3">
         <f t="shared" si="6"/>
         <v>0.47902013793103448</v>
       </c>
-      <c r="R35" s="4">
+      <c r="R35" s="3">
         <f t="shared" si="6"/>
         <v>0.66623673469387756</v>
       </c>
-      <c r="S35" s="4">
+      <c r="S35" s="3">
         <f t="shared" si="6"/>
         <v>1.1342220659340658</v>
       </c>
-      <c r="T35" s="4">
+      <c r="T35" s="3">
         <f t="shared" si="9"/>
         <v>15.125742450363196</v>
       </c>
-      <c r="U35" s="4">
+      <c r="U35" s="3">
         <f t="shared" si="7"/>
         <v>21.845131743842366</v>
       </c>
-      <c r="V35" s="4">
+      <c r="V35" s="3">
         <f t="shared" si="7"/>
         <v>32.902670979591839</v>
       </c>
-      <c r="W35" s="4">
+      <c r="W35" s="3">
         <f t="shared" si="7"/>
         <v>64.623244747252741</v>
       </c>
@@ -5480,36 +5495,36 @@
       <c r="A37" t="s">
         <v>218</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D37" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2" t="s">
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2" t="s">
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2" t="s">
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="Q37" s="2"/>
-      <c r="R37" s="2"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2" t="s">
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="U37" s="2"/>
-      <c r="V37" s="2"/>
-      <c r="W37" s="2"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="4"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
@@ -5628,35 +5643,35 @@
       <c r="O39" t="s">
         <v>32</v>
       </c>
-      <c r="P39" s="4">
+      <c r="P39" s="3">
         <f>H39/D39</f>
         <v>6.0519828571428569</v>
       </c>
-      <c r="Q39" s="4">
+      <c r="Q39" s="3">
         <f t="shared" ref="Q39:S52" si="10">I39/E39</f>
         <v>5.9825638095238096</v>
       </c>
-      <c r="R39" s="4">
+      <c r="R39" s="3">
         <f t="shared" si="10"/>
         <v>4.9088063492063494</v>
       </c>
-      <c r="S39" s="4">
+      <c r="S39" s="3">
         <f t="shared" si="10"/>
         <v>5.294505882352941</v>
       </c>
-      <c r="T39" s="4">
+      <c r="T39" s="3">
         <f>L39/D39</f>
         <v>0</v>
       </c>
-      <c r="U39" s="4">
+      <c r="U39" s="3">
         <f t="shared" ref="U39:W52" si="11">M39/E39</f>
         <v>0</v>
       </c>
-      <c r="V39" s="4">
+      <c r="V39" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W39" s="4">
+      <c r="W39" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -5707,35 +5722,35 @@
       <c r="O40" t="s">
         <v>32</v>
       </c>
-      <c r="P40" s="4">
+      <c r="P40" s="3">
         <f t="shared" ref="P40:P52" si="12">H40/D40</f>
         <v>14.446222996515679</v>
       </c>
-      <c r="Q40" s="4">
+      <c r="Q40" s="3">
         <f t="shared" si="10"/>
         <v>11.075304529616725</v>
       </c>
-      <c r="R40" s="4">
+      <c r="R40" s="3">
         <f t="shared" si="10"/>
         <v>10.284181818181818</v>
       </c>
-      <c r="S40" s="4">
+      <c r="S40" s="3">
         <f t="shared" si="10"/>
         <v>10.494666666666667</v>
       </c>
-      <c r="T40" s="4">
+      <c r="T40" s="3">
         <f t="shared" ref="T40:T52" si="13">L40/D40</f>
         <v>0</v>
       </c>
-      <c r="U40" s="4">
+      <c r="U40" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V40" s="4">
+      <c r="V40" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W40" s="4">
+      <c r="W40" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -5786,35 +5801,35 @@
       <c r="O41" t="s">
         <v>32</v>
       </c>
-      <c r="P41" s="4">
+      <c r="P41" s="3">
         <f t="shared" si="12"/>
         <v>11.036007426226304</v>
       </c>
-      <c r="Q41" s="4">
+      <c r="Q41" s="3">
         <f t="shared" si="10"/>
         <v>7.6195902439024392</v>
       </c>
-      <c r="R41" s="4">
+      <c r="R41" s="3">
         <f t="shared" si="10"/>
         <v>7.4073496598639457</v>
       </c>
-      <c r="S41" s="4">
+      <c r="S41" s="3">
         <f t="shared" si="10"/>
         <v>7.2955102040816326</v>
       </c>
-      <c r="T41" s="4">
+      <c r="T41" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U41" s="4">
+      <c r="U41" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V41" s="4">
+      <c r="V41" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W41" s="4">
+      <c r="W41" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -5865,35 +5880,35 @@
       <c r="O42" t="s">
         <v>32</v>
       </c>
-      <c r="P42" s="4">
+      <c r="P42" s="3">
         <f t="shared" si="12"/>
         <v>7.1783430188334805</v>
       </c>
-      <c r="Q42" s="4">
+      <c r="Q42" s="3">
         <f t="shared" si="10"/>
         <v>5.7737523992322455</v>
       </c>
-      <c r="R42" s="4">
+      <c r="R42" s="3">
         <f t="shared" si="10"/>
         <v>4.9763559183673474</v>
       </c>
-      <c r="S42" s="4">
+      <c r="S42" s="3">
         <f t="shared" si="10"/>
         <v>4.429492711370262</v>
       </c>
-      <c r="T42" s="4">
+      <c r="T42" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U42" s="4">
+      <c r="U42" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V42" s="4">
+      <c r="V42" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W42" s="4">
+      <c r="W42" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -5944,35 +5959,35 @@
       <c r="O43" t="s">
         <v>32</v>
       </c>
-      <c r="P43" s="4">
+      <c r="P43" s="3">
         <f t="shared" si="12"/>
         <v>9.24600382024731</v>
       </c>
-      <c r="Q43" s="4">
+      <c r="Q43" s="3">
         <f t="shared" si="10"/>
         <v>10.789782723434202</v>
       </c>
-      <c r="R43" s="4">
+      <c r="R43" s="3">
         <f t="shared" si="10"/>
         <v>10.535632791295367</v>
       </c>
-      <c r="S43" s="4">
+      <c r="S43" s="3">
         <f t="shared" si="10"/>
         <v>10.313459275094276</v>
       </c>
-      <c r="T43" s="4">
+      <c r="T43" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U43" s="4">
+      <c r="U43" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V43" s="4">
+      <c r="V43" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W43" s="4">
+      <c r="W43" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6023,35 +6038,35 @@
       <c r="O44" t="s">
         <v>32</v>
       </c>
-      <c r="P44" s="4">
+      <c r="P44" s="3">
         <f t="shared" si="12"/>
         <v>11.359398496240601</v>
       </c>
-      <c r="Q44" s="4">
+      <c r="Q44" s="3">
         <f t="shared" si="10"/>
         <v>9.147413793103448</v>
       </c>
-      <c r="R44" s="4">
+      <c r="R44" s="3">
         <f t="shared" si="10"/>
         <v>9.6827586206896559</v>
       </c>
-      <c r="S44" s="4">
+      <c r="S44" s="3">
         <f t="shared" si="10"/>
         <v>9.7631661442006266</v>
       </c>
-      <c r="T44" s="4">
+      <c r="T44" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U44" s="4">
+      <c r="U44" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V44" s="4">
+      <c r="V44" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W44" s="4">
+      <c r="W44" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6102,35 +6117,35 @@
       <c r="O45" t="s">
         <v>32</v>
       </c>
-      <c r="P45" s="4">
+      <c r="P45" s="3">
         <f t="shared" si="12"/>
         <v>54.441873435768734</v>
       </c>
-      <c r="Q45" s="4">
+      <c r="Q45" s="3">
         <f t="shared" si="10"/>
         <v>35.230245164173255</v>
       </c>
-      <c r="R45" s="4">
+      <c r="R45" s="3">
         <f t="shared" si="10"/>
         <v>27.831407849293562</v>
       </c>
-      <c r="S45" s="4">
+      <c r="S45" s="3">
         <f t="shared" si="10"/>
         <v>21.380084144427002</v>
       </c>
-      <c r="T45" s="4">
+      <c r="T45" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U45" s="4">
+      <c r="U45" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V45" s="4">
+      <c r="V45" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W45" s="4">
+      <c r="W45" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6181,35 +6196,35 @@
       <c r="O46" t="s">
         <v>32</v>
       </c>
-      <c r="P46" s="4">
+      <c r="P46" s="3">
         <f t="shared" si="12"/>
         <v>37.246454810495628</v>
       </c>
-      <c r="Q46" s="4">
+      <c r="Q46" s="3">
         <f t="shared" si="10"/>
         <v>25.228915451895045</v>
       </c>
-      <c r="R46" s="4">
+      <c r="R46" s="3">
         <f t="shared" si="10"/>
         <v>18.89391253644315</v>
       </c>
-      <c r="S46" s="4">
+      <c r="S46" s="3">
         <f t="shared" si="10"/>
         <v>12.33552380952381</v>
       </c>
-      <c r="T46" s="4">
+      <c r="T46" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U46" s="4">
+      <c r="U46" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V46" s="4">
+      <c r="V46" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W46" s="4">
+      <c r="W46" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6260,35 +6275,35 @@
       <c r="O47" t="s">
         <v>32</v>
       </c>
-      <c r="P47" s="4">
+      <c r="P47" s="3">
         <f t="shared" si="12"/>
         <v>20.372605357142856</v>
       </c>
-      <c r="Q47" s="4">
+      <c r="Q47" s="3">
         <f t="shared" si="10"/>
         <v>13.232730952380953</v>
       </c>
-      <c r="R47" s="4">
+      <c r="R47" s="3">
         <f t="shared" si="10"/>
         <v>9.6004071428571436</v>
       </c>
-      <c r="S47" s="4">
+      <c r="S47" s="3">
         <f t="shared" si="10"/>
         <v>8.8243714285714283</v>
       </c>
-      <c r="T47" s="4">
+      <c r="T47" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U47" s="4">
+      <c r="U47" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V47" s="4">
+      <c r="V47" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W47" s="4">
+      <c r="W47" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6339,35 +6354,35 @@
       <c r="O48" t="s">
         <v>32</v>
       </c>
-      <c r="P48" s="4">
+      <c r="P48" s="3">
         <f t="shared" si="12"/>
         <v>22.586353568072262</v>
       </c>
-      <c r="Q48" s="4">
+      <c r="Q48" s="3">
         <f t="shared" si="10"/>
         <v>14.846024630541871</v>
       </c>
-      <c r="R48" s="4">
+      <c r="R48" s="3">
         <f t="shared" si="10"/>
         <v>11.570586206896552</v>
       </c>
-      <c r="S48" s="4">
+      <c r="S48" s="3">
         <f t="shared" si="10"/>
         <v>9.8518105263157896</v>
       </c>
-      <c r="T48" s="4">
+      <c r="T48" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U48" s="4">
+      <c r="U48" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V48" s="4">
+      <c r="V48" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W48" s="4">
+      <c r="W48" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6418,35 +6433,35 @@
       <c r="O49" t="s">
         <v>32</v>
       </c>
-      <c r="P49" s="4">
+      <c r="P49" s="3">
         <f t="shared" si="12"/>
         <v>25.28416770180727</v>
       </c>
-      <c r="Q49" s="4">
+      <c r="Q49" s="3">
         <f t="shared" si="10"/>
         <v>15.805057142857143</v>
       </c>
-      <c r="R49" s="4">
+      <c r="R49" s="3">
         <f t="shared" si="10"/>
         <v>11.815164179104478</v>
       </c>
-      <c r="S49" s="4">
+      <c r="S49" s="3">
         <f t="shared" si="10"/>
         <v>10.304146320346319</v>
       </c>
-      <c r="T49" s="4">
+      <c r="T49" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U49" s="4">
+      <c r="U49" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V49" s="4">
+      <c r="V49" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W49" s="4">
+      <c r="W49" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6497,35 +6512,35 @@
       <c r="O50" t="s">
         <v>32</v>
       </c>
-      <c r="P50" s="4">
+      <c r="P50" s="3">
         <f t="shared" si="12"/>
         <v>36.877244444444443</v>
       </c>
-      <c r="Q50" s="4">
+      <c r="Q50" s="3">
         <f t="shared" si="10"/>
         <v>23.023778306878306</v>
       </c>
-      <c r="R50" s="4">
+      <c r="R50" s="3">
         <f t="shared" si="10"/>
         <v>17.515777777777778</v>
       </c>
-      <c r="S50" s="4">
+      <c r="S50" s="3">
         <f t="shared" si="10"/>
         <v>14.284313227513227</v>
       </c>
-      <c r="T50" s="4">
+      <c r="T50" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U50" s="4">
+      <c r="U50" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V50" s="4">
+      <c r="V50" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W50" s="4">
+      <c r="W50" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6576,35 +6591,35 @@
       <c r="O51" t="s">
         <v>32</v>
       </c>
-      <c r="P51" s="4">
+      <c r="P51" s="3">
         <f t="shared" si="12"/>
         <v>38.425642033542978</v>
       </c>
-      <c r="Q51" s="4">
+      <c r="Q51" s="3">
         <f t="shared" si="10"/>
         <v>27.596808163265305</v>
       </c>
-      <c r="R51" s="4">
+      <c r="R51" s="3">
         <f t="shared" si="10"/>
         <v>20.197665995975854</v>
       </c>
-      <c r="S51" s="4">
+      <c r="S51" s="3">
         <f t="shared" si="10"/>
         <v>16.307683702213279</v>
       </c>
-      <c r="T51" s="4">
+      <c r="T51" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U51" s="4">
+      <c r="U51" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V51" s="4">
+      <c r="V51" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W51" s="4">
+      <c r="W51" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6655,35 +6670,35 @@
       <c r="O52" t="s">
         <v>32</v>
       </c>
-      <c r="P52" s="4">
+      <c r="P52" s="3">
         <f t="shared" si="12"/>
         <v>37.546845481049566</v>
       </c>
-      <c r="Q52" s="4">
+      <c r="Q52" s="3">
         <f t="shared" si="10"/>
         <v>23.540767346938775</v>
       </c>
-      <c r="R52" s="4">
+      <c r="R52" s="3">
         <f t="shared" si="10"/>
         <v>17.75411078717201</v>
       </c>
-      <c r="S52" s="4">
+      <c r="S52" s="3">
         <f t="shared" si="10"/>
         <v>14.455771428571429</v>
       </c>
-      <c r="T52" s="4">
+      <c r="T52" s="3">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="U52" s="4">
+      <c r="U52" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="V52" s="4">
+      <c r="V52" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="W52" s="4">
+      <c r="W52" s="3">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
@@ -6692,36 +6707,36 @@
       <c r="A54" t="s">
         <v>219</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="D54" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2" t="s">
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2" t="s">
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="4"/>
+      <c r="L54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2" t="s">
+      <c r="M54" s="4"/>
+      <c r="N54" s="4"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
-      <c r="S54" s="2"/>
-      <c r="T54" s="2" t="s">
+      <c r="Q54" s="4"/>
+      <c r="R54" s="4"/>
+      <c r="S54" s="4"/>
+      <c r="T54" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="U54" s="2"/>
-      <c r="V54" s="2"/>
-      <c r="W54" s="2"/>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="4"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
@@ -6840,35 +6855,35 @@
       <c r="O56" t="s">
         <v>32</v>
       </c>
-      <c r="P56" s="4">
+      <c r="P56" s="3">
         <f>H56/D56</f>
         <v>1.3</v>
       </c>
-      <c r="Q56" s="4">
+      <c r="Q56" s="3">
         <f t="shared" ref="Q56:S69" si="14">I56/E56</f>
         <v>1.3666666666666667</v>
       </c>
-      <c r="R56" s="4">
+      <c r="R56" s="3">
         <f t="shared" si="14"/>
         <v>1.1388888888888888</v>
       </c>
-      <c r="S56" s="4">
+      <c r="S56" s="3">
         <f t="shared" si="14"/>
         <v>1.2352941176470589</v>
       </c>
-      <c r="T56" s="4">
+      <c r="T56" s="3">
         <f>L56/D56</f>
         <v>0</v>
       </c>
-      <c r="U56" s="4">
+      <c r="U56" s="3">
         <f t="shared" ref="U56:W69" si="15">M56/E56</f>
         <v>0</v>
       </c>
-      <c r="V56" s="4">
+      <c r="V56" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W56" s="4">
+      <c r="W56" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -6919,35 +6934,35 @@
       <c r="O57" t="s">
         <v>32</v>
       </c>
-      <c r="P57" s="4">
+      <c r="P57" s="3">
         <f t="shared" ref="P57:P69" si="16">H57/D57</f>
         <v>1.3902439024390243</v>
       </c>
-      <c r="Q57" s="4">
+      <c r="Q57" s="3">
         <f t="shared" si="14"/>
         <v>1.4878048780487805</v>
       </c>
-      <c r="R57" s="4">
+      <c r="R57" s="3">
         <f t="shared" si="14"/>
         <v>1.4772727272727273</v>
       </c>
-      <c r="S57" s="4">
+      <c r="S57" s="3">
         <f t="shared" si="14"/>
         <v>1.5555555555555556</v>
       </c>
-      <c r="T57" s="4">
+      <c r="T57" s="3">
         <f t="shared" ref="T57:T69" si="17">L57/D57</f>
         <v>0</v>
       </c>
-      <c r="U57" s="4">
+      <c r="U57" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V57" s="4">
+      <c r="V57" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W57" s="4">
+      <c r="W57" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -6998,35 +7013,35 @@
       <c r="O58" t="s">
         <v>32</v>
       </c>
-      <c r="P58" s="4">
+      <c r="P58" s="3">
         <f t="shared" si="16"/>
         <v>1.5714285714285714</v>
       </c>
-      <c r="Q58" s="4">
+      <c r="Q58" s="3">
         <f t="shared" si="14"/>
         <v>1.3658536585365855</v>
       </c>
-      <c r="R58" s="4">
+      <c r="R58" s="3">
         <f t="shared" si="14"/>
         <v>1.4047619047619047</v>
       </c>
-      <c r="S58" s="4">
+      <c r="S58" s="3">
         <f t="shared" si="14"/>
         <v>1.4285714285714286</v>
       </c>
-      <c r="T58" s="4">
+      <c r="T58" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U58" s="4">
+      <c r="U58" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V58" s="4">
+      <c r="V58" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W58" s="4">
+      <c r="W58" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7077,35 +7092,35 @@
       <c r="O59" t="s">
         <v>32</v>
       </c>
-      <c r="P59" s="4">
+      <c r="P59" s="3">
         <f t="shared" si="16"/>
         <v>0.82608695652173914</v>
       </c>
-      <c r="Q59" s="4">
+      <c r="Q59" s="3">
         <f t="shared" si="14"/>
         <v>0.75</v>
       </c>
-      <c r="R59" s="4">
+      <c r="R59" s="3">
         <f t="shared" si="14"/>
         <v>0.76</v>
       </c>
-      <c r="S59" s="4">
+      <c r="S59" s="3">
         <f t="shared" si="14"/>
         <v>0.6785714285714286</v>
       </c>
-      <c r="T59" s="4">
+      <c r="T59" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U59" s="4">
+      <c r="U59" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V59" s="4">
+      <c r="V59" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W59" s="4">
+      <c r="W59" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7156,35 +7171,35 @@
       <c r="O60" t="s">
         <v>32</v>
       </c>
-      <c r="P60" s="4">
+      <c r="P60" s="3">
         <f t="shared" si="16"/>
         <v>0.68965517241379315</v>
       </c>
-      <c r="Q60" s="4">
+      <c r="Q60" s="3">
         <f t="shared" si="14"/>
         <v>0.81034482758620685</v>
       </c>
-      <c r="R60" s="4">
+      <c r="R60" s="3">
         <f t="shared" si="14"/>
         <v>0.77419354838709675</v>
       </c>
-      <c r="S60" s="4">
+      <c r="S60" s="3">
         <f t="shared" si="14"/>
         <v>0.75806451612903225</v>
       </c>
-      <c r="T60" s="4">
+      <c r="T60" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U60" s="4">
+      <c r="U60" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V60" s="4">
+      <c r="V60" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W60" s="4">
+      <c r="W60" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7235,35 +7250,35 @@
       <c r="O61" t="s">
         <v>32</v>
       </c>
-      <c r="P61" s="4">
+      <c r="P61" s="3">
         <f t="shared" si="16"/>
         <v>1.4210526315789473</v>
       </c>
-      <c r="Q61" s="4">
+      <c r="Q61" s="3">
         <f t="shared" si="14"/>
         <v>1.125</v>
       </c>
-      <c r="R61" s="4">
+      <c r="R61" s="3">
         <f t="shared" si="14"/>
         <v>1.125</v>
       </c>
-      <c r="S61" s="4">
+      <c r="S61" s="3">
         <f t="shared" si="14"/>
         <v>1.2272727272727273</v>
       </c>
-      <c r="T61" s="4">
+      <c r="T61" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U61" s="4">
+      <c r="U61" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V61" s="4">
+      <c r="V61" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W61" s="4">
+      <c r="W61" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7314,35 +7329,35 @@
       <c r="O62" t="s">
         <v>32</v>
       </c>
-      <c r="P62" s="4">
+      <c r="P62" s="3">
         <f t="shared" si="16"/>
         <v>1.2891566265060241</v>
       </c>
-      <c r="Q62" s="4">
+      <c r="Q62" s="3">
         <f t="shared" si="14"/>
         <v>1.5180722891566265</v>
       </c>
-      <c r="R62" s="4">
+      <c r="R62" s="3">
         <f t="shared" si="14"/>
         <v>1.5494505494505495</v>
       </c>
-      <c r="S62" s="4">
+      <c r="S62" s="3">
         <f t="shared" si="14"/>
         <v>1.6043956043956045</v>
       </c>
-      <c r="T62" s="4">
+      <c r="T62" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U62" s="4">
+      <c r="U62" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V62" s="4">
+      <c r="V62" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W62" s="4">
+      <c r="W62" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7393,35 +7408,35 @@
       <c r="O63" t="s">
         <v>32</v>
       </c>
-      <c r="P63" s="4">
+      <c r="P63" s="3">
         <f t="shared" si="16"/>
         <v>1.7346938775510203</v>
       </c>
-      <c r="Q63" s="4">
+      <c r="Q63" s="3">
         <f t="shared" si="14"/>
         <v>1.8367346938775511</v>
       </c>
-      <c r="R63" s="4">
+      <c r="R63" s="3">
         <f t="shared" si="14"/>
         <v>1.8979591836734695</v>
       </c>
-      <c r="S63" s="4">
+      <c r="S63" s="3">
         <f t="shared" si="14"/>
         <v>1.5833333333333333</v>
       </c>
-      <c r="T63" s="4">
+      <c r="T63" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U63" s="4">
+      <c r="U63" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V63" s="4">
+      <c r="V63" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W63" s="4">
+      <c r="W63" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7472,35 +7487,35 @@
       <c r="O64" t="s">
         <v>32</v>
       </c>
-      <c r="P64" s="4">
+      <c r="P64" s="3">
         <f t="shared" si="16"/>
         <v>1.5208333333333333</v>
       </c>
-      <c r="Q64" s="4">
+      <c r="Q64" s="3">
         <f t="shared" si="14"/>
         <v>1.5833333333333333</v>
       </c>
-      <c r="R64" s="4">
+      <c r="R64" s="3">
         <f t="shared" si="14"/>
         <v>1.625</v>
       </c>
-      <c r="S64" s="4">
+      <c r="S64" s="3">
         <f t="shared" si="14"/>
         <v>1.6875</v>
       </c>
-      <c r="T64" s="4">
+      <c r="T64" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U64" s="4">
+      <c r="U64" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V64" s="4">
+      <c r="V64" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W64" s="4">
+      <c r="W64" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7551,35 +7566,35 @@
       <c r="O65" t="s">
         <v>32</v>
       </c>
-      <c r="P65" s="4">
+      <c r="P65" s="3">
         <f t="shared" si="16"/>
         <v>1.5283018867924529</v>
       </c>
-      <c r="Q65" s="4">
+      <c r="Q65" s="3">
         <f t="shared" si="14"/>
         <v>1.4655172413793103</v>
       </c>
-      <c r="R65" s="4">
+      <c r="R65" s="3">
         <f t="shared" si="14"/>
         <v>1.5517241379310345</v>
       </c>
-      <c r="S65" s="4">
+      <c r="S65" s="3">
         <f t="shared" si="14"/>
         <v>1.5964912280701755</v>
       </c>
-      <c r="T65" s="4">
+      <c r="T65" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U65" s="4">
+      <c r="U65" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V65" s="4">
+      <c r="V65" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W65" s="4">
+      <c r="W65" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7630,35 +7645,35 @@
       <c r="O66" t="s">
         <v>32</v>
       </c>
-      <c r="P66" s="4">
+      <c r="P66" s="3">
         <f t="shared" si="16"/>
         <v>1.6842105263157894</v>
       </c>
-      <c r="Q66" s="4">
+      <c r="Q66" s="3">
         <f t="shared" si="14"/>
         <v>1.5074626865671641</v>
       </c>
-      <c r="R66" s="4">
+      <c r="R66" s="3">
         <f t="shared" si="14"/>
         <v>1.5671641791044777</v>
       </c>
-      <c r="S66" s="4">
+      <c r="S66" s="3">
         <f t="shared" si="14"/>
         <v>1.6212121212121211</v>
       </c>
-      <c r="T66" s="4">
+      <c r="T66" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U66" s="4">
+      <c r="U66" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V66" s="4">
+      <c r="V66" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W66" s="4">
+      <c r="W66" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7709,35 +7724,35 @@
       <c r="O67" t="s">
         <v>32</v>
       </c>
-      <c r="P67" s="4">
+      <c r="P67" s="3">
         <f t="shared" si="16"/>
         <v>1.8148148148148149</v>
       </c>
-      <c r="Q67" s="4">
+      <c r="Q67" s="3">
         <f t="shared" si="14"/>
         <v>1.8703703703703705</v>
       </c>
-      <c r="R67" s="4">
+      <c r="R67" s="3">
         <f t="shared" si="14"/>
         <v>1.9444444444444444</v>
       </c>
-      <c r="S67" s="4">
+      <c r="S67" s="3">
         <f t="shared" si="14"/>
         <v>1.962962962962963</v>
       </c>
-      <c r="T67" s="4">
+      <c r="T67" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U67" s="4">
+      <c r="U67" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V67" s="4">
+      <c r="V67" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W67" s="4">
+      <c r="W67" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7788,35 +7803,35 @@
       <c r="O68" t="s">
         <v>32</v>
       </c>
-      <c r="P68" s="4">
+      <c r="P68" s="3">
         <f t="shared" si="16"/>
         <v>1.7301587301587302</v>
       </c>
-      <c r="Q68" s="4">
+      <c r="Q68" s="3">
         <f t="shared" si="14"/>
         <v>1.6428571428571428</v>
       </c>
-      <c r="R68" s="4">
+      <c r="R68" s="3">
         <f t="shared" si="14"/>
         <v>1.6901408450704225</v>
       </c>
-      <c r="S68" s="4">
+      <c r="S68" s="3">
         <f t="shared" si="14"/>
         <v>1.704225352112676</v>
       </c>
-      <c r="T68" s="4">
+      <c r="T68" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U68" s="4">
+      <c r="U68" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V68" s="4">
+      <c r="V68" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W68" s="4">
+      <c r="W68" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7867,35 +7882,35 @@
       <c r="O69" t="s">
         <v>32</v>
       </c>
-      <c r="P69" s="4">
+      <c r="P69" s="3">
         <f t="shared" si="16"/>
         <v>1.8367346938775511</v>
       </c>
-      <c r="Q69" s="4">
+      <c r="Q69" s="3">
         <f t="shared" si="14"/>
         <v>1.8979591836734695</v>
       </c>
-      <c r="R69" s="4">
+      <c r="R69" s="3">
         <f t="shared" si="14"/>
         <v>1.9795918367346939</v>
       </c>
-      <c r="S69" s="4">
+      <c r="S69" s="3">
         <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="T69" s="4">
+      <c r="T69" s="3">
         <f t="shared" si="17"/>
         <v>0</v>
       </c>
-      <c r="U69" s="4">
+      <c r="U69" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="V69" s="4">
+      <c r="V69" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="W69" s="4">
+      <c r="W69" s="3">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
@@ -7904,36 +7919,36 @@
       <c r="A71" t="s">
         <v>18</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D71" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2" t="s">
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2" t="s">
+      <c r="I71" s="4"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="4"/>
+      <c r="L71" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
-      <c r="O71" s="2"/>
-      <c r="P71" s="2" t="s">
+      <c r="M71" s="4"/>
+      <c r="N71" s="4"/>
+      <c r="O71" s="4"/>
+      <c r="P71" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="Q71" s="2"/>
-      <c r="R71" s="2"/>
-      <c r="S71" s="2"/>
-      <c r="T71" s="2" t="s">
+      <c r="Q71" s="4"/>
+      <c r="R71" s="4"/>
+      <c r="S71" s="4"/>
+      <c r="T71" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="U71" s="2"/>
-      <c r="V71" s="2"/>
-      <c r="W71" s="2"/>
+      <c r="U71" s="4"/>
+      <c r="V71" s="4"/>
+      <c r="W71" s="4"/>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
@@ -8052,35 +8067,35 @@
       <c r="O73" t="s">
         <v>472</v>
       </c>
-      <c r="P73" s="4">
+      <c r="P73" s="3">
         <f>H73/D73</f>
         <v>1.0010905125408942</v>
       </c>
-      <c r="Q73" s="4">
+      <c r="Q73" s="3">
         <f t="shared" ref="Q73:S86" si="18">I73/E73</f>
         <v>1.0010905125408942</v>
       </c>
-      <c r="R73" s="4">
+      <c r="R73" s="3">
         <f t="shared" si="18"/>
         <v>1.0039721425071744</v>
       </c>
-      <c r="S73" s="4">
+      <c r="S73" s="3">
         <f t="shared" si="18"/>
         <v>1.002990242367013</v>
       </c>
-      <c r="T73" s="4">
+      <c r="T73" s="3">
         <f>L73/D73</f>
         <v>0.99127753544165753</v>
       </c>
-      <c r="U73" s="4">
+      <c r="U73" s="3">
         <f t="shared" ref="U73:W86" si="19">M73/E73</f>
         <v>0.99128353326063245</v>
       </c>
-      <c r="V73" s="4">
+      <c r="V73" s="3">
         <f t="shared" si="19"/>
         <v>0.99413748075173236</v>
       </c>
-      <c r="W73" s="4">
+      <c r="W73" s="3">
         <f t="shared" si="19"/>
         <v>1.0016453983492464</v>
       </c>
@@ -8131,35 +8146,35 @@
       <c r="O74" t="s">
         <v>482</v>
       </c>
-      <c r="P74" s="4">
+      <c r="P74" s="3">
         <f t="shared" ref="P74:P86" si="20">H74/D74</f>
         <v>0.99377123442808613</v>
       </c>
-      <c r="Q74" s="4">
+      <c r="Q74" s="3">
         <f t="shared" si="18"/>
         <v>0.99320882852292025</v>
       </c>
-      <c r="R74" s="4">
+      <c r="R74" s="3">
         <f t="shared" si="18"/>
         <v>1.0048036168409156</v>
       </c>
-      <c r="S74" s="4">
+      <c r="S74" s="3">
         <f t="shared" si="18"/>
         <v>0.99934630070728581</v>
       </c>
-      <c r="T74" s="4">
+      <c r="T74" s="3">
         <f t="shared" ref="T74:T86" si="21">L74/D74</f>
         <v>1.0021409022272556</v>
       </c>
-      <c r="U74" s="4">
+      <c r="U74" s="3">
         <f t="shared" si="19"/>
         <v>1.0002758913412564</v>
       </c>
-      <c r="V74" s="4">
+      <c r="V74" s="3">
         <f t="shared" si="19"/>
         <v>1.0002806819252144</v>
       </c>
-      <c r="W74" s="4">
+      <c r="W74" s="3">
         <f t="shared" si="19"/>
         <v>0.99782801629852824</v>
       </c>
@@ -8210,35 +8225,35 @@
       <c r="O75" t="s">
         <v>494</v>
       </c>
-      <c r="P75" s="4">
+      <c r="P75" s="3">
         <f t="shared" si="20"/>
         <v>0.99622641509433962</v>
       </c>
-      <c r="Q75" s="4">
+      <c r="Q75" s="3">
         <f t="shared" si="18"/>
         <v>0.99404761904761907</v>
       </c>
-      <c r="R75" s="4">
+      <c r="R75" s="3">
         <f t="shared" si="18"/>
         <v>0.9967001356001286</v>
       </c>
-      <c r="S75" s="4">
+      <c r="S75" s="3">
         <f t="shared" si="18"/>
         <v>0.99243197416524365</v>
       </c>
-      <c r="T75" s="4">
+      <c r="T75" s="3">
         <f t="shared" si="21"/>
         <v>0.9874292452830189</v>
       </c>
-      <c r="U75" s="4">
+      <c r="U75" s="3">
         <f t="shared" si="19"/>
         <v>1.0024968671679197</v>
       </c>
-      <c r="V75" s="4">
+      <c r="V75" s="3">
         <f t="shared" si="19"/>
         <v>0.99387317338266146</v>
       </c>
-      <c r="W75" s="4">
+      <c r="W75" s="3">
         <f t="shared" si="19"/>
         <v>0.99606485626388952</v>
       </c>
@@ -8289,35 +8304,35 @@
       <c r="O76" t="s">
         <v>505</v>
       </c>
-      <c r="P76" s="4">
+      <c r="P76" s="3">
         <f t="shared" si="20"/>
         <v>0.99185624999999999</v>
       </c>
-      <c r="Q76" s="4">
+      <c r="Q76" s="3">
         <f t="shared" si="18"/>
         <v>0.99878731086183614</v>
       </c>
-      <c r="R76" s="4">
+      <c r="R76" s="3">
         <f t="shared" si="18"/>
         <v>0.99750623441396513</v>
       </c>
-      <c r="S76" s="4">
+      <c r="S76" s="3">
         <f t="shared" si="18"/>
         <v>0.99930118798043321</v>
       </c>
-      <c r="T76" s="4">
+      <c r="T76" s="3">
         <f t="shared" si="21"/>
         <v>0.99999916666666666</v>
       </c>
-      <c r="U76" s="4">
+      <c r="U76" s="3">
         <f t="shared" si="19"/>
         <v>1.0009805076089562</v>
       </c>
-      <c r="V76" s="4">
+      <c r="V76" s="3">
         <f t="shared" si="19"/>
         <v>1.001476080029696</v>
       </c>
-      <c r="W76" s="4">
+      <c r="W76" s="3">
         <f t="shared" si="19"/>
         <v>1.0016355528934144</v>
       </c>
@@ -8368,35 +8383,35 @@
       <c r="O77" t="s">
         <v>516</v>
       </c>
-      <c r="P77" s="4">
+      <c r="P77" s="3">
         <f t="shared" si="20"/>
         <v>0.99709379128137388</v>
       </c>
-      <c r="Q77" s="4">
+      <c r="Q77" s="3">
         <f t="shared" si="18"/>
         <v>0.9997353797300873</v>
       </c>
-      <c r="R77" s="4">
+      <c r="R77" s="3">
         <f t="shared" si="18"/>
         <v>0.99990314554683868</v>
       </c>
-      <c r="S77" s="4">
+      <c r="S77" s="3">
         <f t="shared" si="18"/>
         <v>0.99969860859841353</v>
       </c>
-      <c r="T77" s="4">
+      <c r="T77" s="3">
         <f t="shared" si="21"/>
         <v>0.99947133421400269</v>
       </c>
-      <c r="U77" s="4">
+      <c r="U77" s="3">
         <f t="shared" si="19"/>
         <v>1.0026460703889919</v>
       </c>
-      <c r="V77" s="4">
+      <c r="V77" s="3">
         <f t="shared" si="19"/>
         <v>1.0026817569080249</v>
       </c>
-      <c r="W77" s="4">
+      <c r="W77" s="3">
         <f t="shared" si="19"/>
         <v>1.0002266389248979</v>
       </c>
@@ -8447,35 +8462,35 @@
       <c r="O78" t="s">
         <v>524</v>
       </c>
-      <c r="P78" s="4">
+      <c r="P78" s="3">
         <f t="shared" si="20"/>
         <v>1.019672131147541</v>
       </c>
-      <c r="Q78" s="4">
+      <c r="Q78" s="3">
         <f t="shared" si="18"/>
         <v>0.9985423208563704</v>
       </c>
-      <c r="R78" s="4">
+      <c r="R78" s="3">
         <f t="shared" si="18"/>
         <v>0.9985423208563704</v>
       </c>
-      <c r="S78" s="4">
+      <c r="S78" s="3">
         <f t="shared" si="18"/>
         <v>0.99590111438452666</v>
       </c>
-      <c r="T78" s="4">
+      <c r="T78" s="3">
         <f t="shared" si="21"/>
         <v>1.0131163934426231</v>
       </c>
-      <c r="U78" s="4">
+      <c r="U78" s="3">
         <f t="shared" si="19"/>
         <v>1.0049638148811701</v>
       </c>
-      <c r="V78" s="4">
+      <c r="V78" s="3">
         <f t="shared" si="19"/>
         <v>1.0113826332834597</v>
       </c>
-      <c r="W78" s="4">
+      <c r="W78" s="3">
         <f t="shared" si="19"/>
         <v>1.0087047948422356</v>
       </c>
@@ -8526,35 +8541,35 @@
       <c r="O79" t="s">
         <v>534</v>
       </c>
-      <c r="P79" s="4">
+      <c r="P79" s="3">
         <f t="shared" si="20"/>
         <v>0.99035493827160492</v>
       </c>
-      <c r="Q79" s="4">
+      <c r="Q79" s="3">
         <f t="shared" si="18"/>
         <v>0.99305555555555558</v>
       </c>
-      <c r="R79" s="4">
+      <c r="R79" s="3">
         <f t="shared" si="18"/>
         <v>0.994054054054054</v>
       </c>
-      <c r="S79" s="4">
+      <c r="S79" s="3">
         <f t="shared" si="18"/>
         <v>0.99644787644787647</v>
       </c>
-      <c r="T79" s="4">
+      <c r="T79" s="3">
         <f t="shared" si="21"/>
         <v>0.99228240740740736</v>
       </c>
-      <c r="U79" s="4">
+      <c r="U79" s="3">
         <f t="shared" si="19"/>
         <v>1.0007656893004115</v>
       </c>
-      <c r="V79" s="4">
+      <c r="V79" s="3">
         <f t="shared" si="19"/>
         <v>0.99921621621621626</v>
       </c>
-      <c r="W79" s="4">
+      <c r="W79" s="3">
         <f t="shared" si="19"/>
         <v>0.97836512226512229</v>
       </c>
@@ -8605,35 +8620,35 @@
       <c r="O80" t="s">
         <v>543</v>
       </c>
-      <c r="P80" s="4">
+      <c r="P80" s="3">
         <f t="shared" si="20"/>
         <v>1.0323974082073435</v>
       </c>
-      <c r="Q80" s="4">
+      <c r="Q80" s="3">
         <f t="shared" si="18"/>
         <v>1.0306695464362852</v>
       </c>
-      <c r="R80" s="4">
+      <c r="R80" s="3">
         <f t="shared" si="18"/>
         <v>1.0289416846652268</v>
       </c>
-      <c r="S80" s="4">
+      <c r="S80" s="3">
         <f t="shared" si="18"/>
         <v>1.0142877351817796</v>
       </c>
-      <c r="T80" s="4">
+      <c r="T80" s="3">
         <f t="shared" si="21"/>
         <v>1.0388668106551475</v>
       </c>
-      <c r="U80" s="4">
+      <c r="U80" s="3">
         <f t="shared" si="19"/>
         <v>1.0367008639308855</v>
       </c>
-      <c r="V80" s="4">
+      <c r="V80" s="3">
         <f t="shared" si="19"/>
         <v>1.0367113030957524</v>
       </c>
-      <c r="W80" s="4">
+      <c r="W80" s="3">
         <f t="shared" si="19"/>
         <v>1.0072050502192673</v>
       </c>
@@ -8684,35 +8699,35 @@
       <c r="O81" t="s">
         <v>552</v>
       </c>
-      <c r="P81" s="4">
+      <c r="P81" s="3">
         <f t="shared" si="20"/>
         <v>1.0111987381703471</v>
       </c>
-      <c r="Q81" s="4">
+      <c r="Q81" s="3">
         <f t="shared" si="18"/>
         <v>1.0116719242902208</v>
       </c>
-      <c r="R81" s="4">
+      <c r="R81" s="3">
         <f t="shared" si="18"/>
         <v>1.0059936908517351</v>
       </c>
-      <c r="S81" s="4">
+      <c r="S81" s="3">
         <f t="shared" si="18"/>
         <v>1.0184983677910773</v>
       </c>
-      <c r="T81" s="4">
+      <c r="T81" s="3">
         <f t="shared" si="21"/>
         <v>1.0126163249211357</v>
       </c>
-      <c r="U81" s="4">
+      <c r="U81" s="3">
         <f t="shared" si="19"/>
         <v>1.0220670347003153</v>
       </c>
-      <c r="V81" s="4">
+      <c r="V81" s="3">
         <f t="shared" si="19"/>
         <v>1.0149810725552051</v>
       </c>
-      <c r="W81" s="4">
+      <c r="W81" s="3">
         <f t="shared" si="19"/>
         <v>1.011383519635968</v>
       </c>
@@ -8763,35 +8778,35 @@
       <c r="O82" t="s">
         <v>562</v>
       </c>
-      <c r="P82" s="4">
+      <c r="P82" s="3">
         <f t="shared" si="20"/>
         <v>1.0020640569395018</v>
       </c>
-      <c r="Q82" s="4">
+      <c r="Q82" s="3">
         <f t="shared" si="18"/>
         <v>1.0038461538461538</v>
       </c>
-      <c r="R82" s="4">
+      <c r="R82" s="3">
         <f t="shared" si="18"/>
         <v>1.0038461538461538</v>
       </c>
-      <c r="S82" s="4">
+      <c r="S82" s="3">
         <f t="shared" si="18"/>
         <v>1.0216076058772687</v>
       </c>
-      <c r="T82" s="4">
+      <c r="T82" s="3">
         <f t="shared" si="21"/>
         <v>1.0035519572953737</v>
       </c>
-      <c r="U82" s="4">
+      <c r="U82" s="3">
         <f t="shared" si="19"/>
         <v>1.0105747863247863</v>
       </c>
-      <c r="V82" s="4">
+      <c r="V82" s="3">
         <f t="shared" si="19"/>
         <v>1.008539886039886</v>
       </c>
-      <c r="W82" s="4">
+      <c r="W82" s="3">
         <f t="shared" si="19"/>
         <v>1.0090377412849323</v>
       </c>
@@ -8842,35 +8857,35 @@
       <c r="O83" t="s">
         <v>572</v>
       </c>
-      <c r="P83" s="4">
+      <c r="P83" s="3">
         <f t="shared" si="20"/>
         <v>0.99226450405489708</v>
       </c>
-      <c r="Q83" s="4">
+      <c r="Q83" s="3">
         <f t="shared" si="18"/>
         <v>1.0137667304015296</v>
       </c>
-      <c r="R83" s="4">
+      <c r="R83" s="3">
         <f t="shared" si="18"/>
         <v>1.0149139579349904</v>
       </c>
-      <c r="S83" s="4">
+      <c r="S83" s="3">
         <f t="shared" si="18"/>
         <v>1.0043359050400338</v>
       </c>
-      <c r="T83" s="4">
+      <c r="T83" s="3">
         <f t="shared" si="21"/>
         <v>1.0012426699937618</v>
       </c>
-      <c r="U83" s="4">
+      <c r="U83" s="3">
         <f t="shared" si="19"/>
         <v>1.0229311663479923</v>
       </c>
-      <c r="V83" s="4">
+      <c r="V83" s="3">
         <f t="shared" si="19"/>
         <v>1.019112810707457</v>
       </c>
-      <c r="W83" s="4">
+      <c r="W83" s="3">
         <f t="shared" si="19"/>
         <v>0.98434661594491679</v>
       </c>
@@ -8921,35 +8936,35 @@
       <c r="O84" t="s">
         <v>580</v>
       </c>
-      <c r="P84" s="4">
+      <c r="P84" s="3">
         <f t="shared" si="20"/>
         <v>1.003415559772296</v>
       </c>
-      <c r="Q84" s="4">
+      <c r="Q84" s="3">
         <f t="shared" si="18"/>
         <v>1.0037950664136623</v>
       </c>
-      <c r="R84" s="4">
+      <c r="R84" s="3">
         <f t="shared" si="18"/>
         <v>1.0030360531309297</v>
       </c>
-      <c r="S84" s="4">
+      <c r="S84" s="3">
         <f t="shared" si="18"/>
         <v>1.0060721062618596</v>
       </c>
-      <c r="T84" s="4">
+      <c r="T84" s="3">
         <f t="shared" si="21"/>
         <v>1.0113801391524351</v>
       </c>
-      <c r="U84" s="4">
+      <c r="U84" s="3">
         <f t="shared" si="19"/>
         <v>1.0151676154332701</v>
       </c>
-      <c r="V84" s="4">
+      <c r="V84" s="3">
         <f t="shared" si="19"/>
         <v>1.0132700822264389</v>
       </c>
-      <c r="W84" s="4">
+      <c r="W84" s="3">
         <f t="shared" si="19"/>
         <v>0.99240069576217582</v>
       </c>
@@ -9000,35 +9015,35 @@
       <c r="O85" t="s">
         <v>592</v>
       </c>
-      <c r="P85" s="4">
+      <c r="P85" s="3">
         <f t="shared" si="20"/>
         <v>1.0092307692307692</v>
       </c>
-      <c r="Q85" s="4">
+      <c r="Q85" s="3">
         <f t="shared" si="18"/>
         <v>1.0107244723331432</v>
       </c>
-      <c r="R85" s="4">
+      <c r="R85" s="3">
         <f t="shared" si="18"/>
         <v>1.0077141236528644</v>
       </c>
-      <c r="S85" s="4">
+      <c r="S85" s="3">
         <f t="shared" si="18"/>
         <v>1.0115165336374001</v>
       </c>
-      <c r="T85" s="4">
+      <c r="T85" s="3">
         <f t="shared" si="21"/>
         <v>0.99828490028490025</v>
       </c>
-      <c r="U85" s="4">
+      <c r="U85" s="3">
         <f t="shared" si="19"/>
         <v>1.0148160296634341</v>
       </c>
-      <c r="V85" s="4">
+      <c r="V85" s="3">
         <f t="shared" si="19"/>
         <v>1.007362733976177</v>
       </c>
-      <c r="W85" s="4">
+      <c r="W85" s="3">
         <f t="shared" si="19"/>
         <v>0.97662770809578103</v>
       </c>
@@ -9079,35 +9094,35 @@
       <c r="O86" t="s">
         <v>600</v>
       </c>
-      <c r="P86" s="4">
+      <c r="P86" s="3">
         <f t="shared" si="20"/>
         <v>1.0040404040404041</v>
       </c>
-      <c r="Q86" s="4">
+      <c r="Q86" s="3">
         <f t="shared" si="18"/>
         <v>1.0072727272727273</v>
       </c>
-      <c r="R86" s="4">
+      <c r="R86" s="3">
         <f t="shared" si="18"/>
         <v>1.0040404040404041</v>
       </c>
-      <c r="S86" s="4">
+      <c r="S86" s="3">
         <f t="shared" si="18"/>
         <v>1.0096969696969698</v>
       </c>
-      <c r="T86" s="4">
+      <c r="T86" s="3">
         <f t="shared" si="21"/>
         <v>1.0121181818181819</v>
       </c>
-      <c r="U86" s="4">
+      <c r="U86" s="3">
         <f t="shared" si="19"/>
         <v>1.012106734006734</v>
       </c>
-      <c r="V86" s="4">
+      <c r="V86" s="3">
         <f t="shared" si="19"/>
         <v>1.0090797979797981</v>
       </c>
-      <c r="W86" s="4">
+      <c r="W86" s="3">
         <f t="shared" si="19"/>
         <v>0.99593905723905729</v>
       </c>
@@ -9116,36 +9131,36 @@
       <c r="A88" t="s">
         <v>17</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D88" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2" t="s">
+      <c r="E88" s="4"/>
+      <c r="F88" s="4"/>
+      <c r="G88" s="4"/>
+      <c r="H88" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I88" s="2"/>
-      <c r="J88" s="2"/>
-      <c r="K88" s="2"/>
-      <c r="L88" s="2" t="s">
+      <c r="I88" s="4"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="4"/>
+      <c r="L88" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M88" s="2"/>
-      <c r="N88" s="2"/>
-      <c r="O88" s="2"/>
-      <c r="P88" s="2" t="s">
+      <c r="M88" s="4"/>
+      <c r="N88" s="4"/>
+      <c r="O88" s="4"/>
+      <c r="P88" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="Q88" s="2"/>
-      <c r="R88" s="2"/>
-      <c r="S88" s="2"/>
-      <c r="T88" s="2" t="s">
+      <c r="Q88" s="4"/>
+      <c r="R88" s="4"/>
+      <c r="S88" s="4"/>
+      <c r="T88" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="U88" s="2"/>
-      <c r="V88" s="2"/>
-      <c r="W88" s="2"/>
+      <c r="U88" s="4"/>
+      <c r="V88" s="4"/>
+      <c r="W88" s="4"/>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
@@ -9228,7 +9243,7 @@
       <c r="C90">
         <v>418</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="2" t="s">
         <v>601</v>
       </c>
       <c r="E90" t="s">
@@ -9264,35 +9279,35 @@
       <c r="O90" t="s">
         <v>611</v>
       </c>
-      <c r="P90" s="4">
+      <c r="P90" s="3">
         <f>H90/D90</f>
         <v>0.71601856492368854</v>
       </c>
-      <c r="Q90" s="4">
+      <c r="Q90" s="3">
         <f t="shared" ref="Q90:S103" si="22">I90/E90</f>
         <v>0.38073621445185502</v>
       </c>
-      <c r="R90" s="4">
+      <c r="R90" s="3">
         <f t="shared" si="22"/>
         <v>0.19745523864520004</v>
       </c>
-      <c r="S90" s="4">
+      <c r="S90" s="3">
         <f t="shared" si="22"/>
         <v>0.37419715766543654</v>
       </c>
-      <c r="T90" s="4">
+      <c r="T90" s="3">
         <f>L90/D90</f>
         <v>0.28349096812607355</v>
       </c>
-      <c r="U90" s="4">
+      <c r="U90" s="3">
         <f t="shared" ref="U90:W103" si="23">M90/E90</f>
         <v>0.24857893091055511</v>
       </c>
-      <c r="V90" s="4">
+      <c r="V90" s="3">
         <f t="shared" si="23"/>
         <v>0.18808354359221696</v>
       </c>
-      <c r="W90" s="4">
+      <c r="W90" s="3">
         <f t="shared" si="23"/>
         <v>0.13311819804758249</v>
       </c>
@@ -9343,35 +9358,35 @@
       <c r="O91" t="s">
         <v>621</v>
       </c>
-      <c r="P91" s="4">
+      <c r="P91" s="3">
         <f t="shared" ref="P91:P103" si="24">H91/D91</f>
         <v>0.76988661476401254</v>
       </c>
-      <c r="Q91" s="4">
+      <c r="Q91" s="3">
         <f t="shared" si="22"/>
         <v>0.53734123587535609</v>
       </c>
-      <c r="R91" s="4">
+      <c r="R91" s="3">
         <f t="shared" si="22"/>
         <v>0.28729003033524003</v>
       </c>
-      <c r="S91" s="4">
+      <c r="S91" s="3">
         <f t="shared" si="22"/>
         <v>0.15202395286380679</v>
       </c>
-      <c r="T91" s="4">
+      <c r="T91" s="3">
         <f t="shared" ref="T91:T103" si="25">L91/D91</f>
         <v>0.30651636313459835</v>
       </c>
-      <c r="U91" s="4">
+      <c r="U91" s="3">
         <f t="shared" si="23"/>
         <v>0.21801486362078148</v>
       </c>
-      <c r="V91" s="4">
+      <c r="V91" s="3">
         <f t="shared" si="23"/>
         <v>0.15966103010454555</v>
       </c>
-      <c r="W91" s="4">
+      <c r="W91" s="3">
         <f t="shared" si="23"/>
         <v>0.1030125723788011</v>
       </c>
@@ -9422,35 +9437,35 @@
       <c r="O92" t="s">
         <v>633</v>
       </c>
-      <c r="P92" s="4">
+      <c r="P92" s="3">
         <f t="shared" si="24"/>
         <v>0.71195496736954322</v>
       </c>
-      <c r="Q92" s="4">
+      <c r="Q92" s="3">
         <f t="shared" si="22"/>
         <v>0.47801443643838765</v>
       </c>
-      <c r="R92" s="4">
+      <c r="R92" s="3">
         <f t="shared" si="22"/>
         <v>0.26157822206763559</v>
       </c>
-      <c r="S92" s="4">
+      <c r="S92" s="3">
         <f t="shared" si="22"/>
         <v>0.58656031571199629</v>
       </c>
-      <c r="T92" s="4">
+      <c r="T92" s="3">
         <f t="shared" si="25"/>
         <v>0.15237713327986593</v>
       </c>
-      <c r="U92" s="4">
+      <c r="U92" s="3">
         <f t="shared" si="23"/>
         <v>0.11459029370831755</v>
       </c>
-      <c r="V92" s="4">
+      <c r="V92" s="3">
         <f t="shared" si="23"/>
         <v>7.0625063290024617E-2</v>
       </c>
-      <c r="W92" s="4">
+      <c r="W92" s="3">
         <f t="shared" si="23"/>
         <v>5.2534100340872907E-2</v>
       </c>
@@ -9501,35 +9516,35 @@
       <c r="O93" t="s">
         <v>645</v>
       </c>
-      <c r="P93" s="4">
+      <c r="P93" s="3">
         <f t="shared" si="24"/>
         <v>0.74802307800778667</v>
       </c>
-      <c r="Q93" s="4">
+      <c r="Q93" s="3">
         <f t="shared" si="22"/>
         <v>0.48247862521289775</v>
       </c>
-      <c r="R93" s="4">
+      <c r="R93" s="3">
         <f t="shared" si="22"/>
         <v>0.30544473437913822</v>
       </c>
-      <c r="S93" s="4">
+      <c r="S93" s="3">
         <f t="shared" si="22"/>
         <v>0.15932125644154546</v>
       </c>
-      <c r="T93" s="4">
+      <c r="T93" s="3">
         <f t="shared" si="25"/>
         <v>0.15893082698194744</v>
       </c>
-      <c r="U93" s="4">
+      <c r="U93" s="3">
         <f t="shared" si="23"/>
         <v>0.121067954271107</v>
       </c>
-      <c r="V93" s="4">
+      <c r="V93" s="3">
         <f t="shared" si="23"/>
         <v>0.11648234769020062</v>
       </c>
-      <c r="W93" s="4">
+      <c r="W93" s="3">
         <f t="shared" si="23"/>
         <v>7.4737290293128728E-2</v>
       </c>
@@ -9580,35 +9595,35 @@
       <c r="O94" t="s">
         <v>655</v>
       </c>
-      <c r="P94" s="4">
+      <c r="P94" s="3">
         <f t="shared" si="24"/>
         <v>0.29835801281346069</v>
       </c>
-      <c r="Q94" s="4">
+      <c r="Q94" s="3">
         <f t="shared" si="22"/>
         <v>0.15020612349807877</v>
       </c>
-      <c r="R94" s="4">
+      <c r="R94" s="3">
         <f t="shared" si="22"/>
         <v>8.0164125960907953E-2</v>
       </c>
-      <c r="S94" s="4">
+      <c r="S94" s="3">
         <f t="shared" si="22"/>
         <v>4.0092742702012268E-2</v>
       </c>
-      <c r="T94" s="4">
+      <c r="T94" s="3">
         <f t="shared" si="25"/>
         <v>0.14944103627813571</v>
       </c>
-      <c r="U94" s="4">
+      <c r="U94" s="3">
         <f t="shared" si="23"/>
         <v>8.9745230956329011E-2</v>
       </c>
-      <c r="V94" s="4">
+      <c r="V94" s="3">
         <f t="shared" si="23"/>
         <v>5.763845725014257E-2</v>
       </c>
-      <c r="W94" s="4">
+      <c r="W94" s="3">
         <f t="shared" si="23"/>
         <v>3.0316525587544881E-2</v>
       </c>
@@ -9659,35 +9674,35 @@
       <c r="O95" t="s">
         <v>666</v>
       </c>
-      <c r="P95" s="4">
+      <c r="P95" s="3">
         <f t="shared" si="24"/>
         <v>0.12509952648457415</v>
       </c>
-      <c r="Q95" s="4">
+      <c r="Q95" s="3">
         <f t="shared" si="22"/>
         <v>7.0277096954919377E-2</v>
       </c>
-      <c r="R95" s="4">
+      <c r="R95" s="3">
         <f t="shared" si="22"/>
         <v>3.3196137123057717E-2</v>
       </c>
-      <c r="S95" s="4">
+      <c r="S95" s="3">
         <f t="shared" si="22"/>
         <v>4.2432492816726508E-2</v>
       </c>
-      <c r="T95" s="4">
+      <c r="T95" s="3">
         <f t="shared" si="25"/>
         <v>0.14111802587588318</v>
       </c>
-      <c r="U95" s="4">
+      <c r="U95" s="3">
         <f t="shared" si="23"/>
         <v>8.4884747797773968E-2</v>
       </c>
-      <c r="V95" s="4">
+      <c r="V95" s="3">
         <f t="shared" si="23"/>
         <v>6.5228515569360754E-2</v>
       </c>
-      <c r="W95" s="4">
+      <c r="W95" s="3">
         <f t="shared" si="23"/>
         <v>5.3247151370927101E-2</v>
       </c>
@@ -9738,35 +9753,35 @@
       <c r="O96" t="s">
         <v>676</v>
       </c>
-      <c r="P96" s="4">
+      <c r="P96" s="3">
         <f t="shared" si="24"/>
         <v>0.94718047180471798</v>
       </c>
-      <c r="Q96" s="4">
+      <c r="Q96" s="3">
         <f t="shared" si="22"/>
         <v>0.86180061800618002</v>
       </c>
-      <c r="R96" s="4">
+      <c r="R96" s="3">
         <f t="shared" si="22"/>
         <v>0.74230309911048509</v>
       </c>
-      <c r="S96" s="4">
+      <c r="S96" s="3">
         <f t="shared" si="22"/>
         <v>0.50027686886483769</v>
       </c>
-      <c r="T96" s="4">
+      <c r="T96" s="3">
         <f t="shared" si="25"/>
         <v>0.15357953579535794</v>
       </c>
-      <c r="U96" s="4">
+      <c r="U96" s="3">
         <f t="shared" si="23"/>
         <v>8.0745807458074581E-2</v>
       </c>
-      <c r="V96" s="4">
+      <c r="V96" s="3">
         <f t="shared" si="23"/>
         <v>5.3020655381270383E-2</v>
       </c>
-      <c r="W96" s="4">
+      <c r="W96" s="3">
         <f t="shared" si="23"/>
         <v>3.1825460153911245E-2</v>
       </c>
@@ -9817,35 +9832,35 @@
       <c r="O97" t="s">
         <v>686</v>
       </c>
-      <c r="P97" s="4">
+      <c r="P97" s="3">
         <f t="shared" si="24"/>
         <v>0.93146731139331029</v>
       </c>
-      <c r="Q97" s="4">
+      <c r="Q97" s="3">
         <f t="shared" si="22"/>
         <v>0.72802701111454748</v>
       </c>
-      <c r="R97" s="4">
+      <c r="R97" s="3">
         <f t="shared" si="22"/>
         <v>0.50226719507947259</v>
       </c>
-      <c r="S97" s="4">
+      <c r="S97" s="3">
         <f t="shared" si="22"/>
         <v>0.34228114361871192</v>
       </c>
-      <c r="T97" s="4">
+      <c r="T97" s="3">
         <f t="shared" si="25"/>
         <v>6.7252414385514603E-2</v>
       </c>
-      <c r="U97" s="4">
+      <c r="U97" s="3">
         <f t="shared" si="23"/>
         <v>4.6789604502126429E-2</v>
       </c>
-      <c r="V97" s="4">
+      <c r="V97" s="3">
         <f t="shared" si="23"/>
         <v>3.3169993906881114E-2</v>
       </c>
-      <c r="W97" s="4">
+      <c r="W97" s="3">
         <f t="shared" si="23"/>
         <v>1.9168085997181068E-2</v>
       </c>
@@ -9896,35 +9911,35 @@
       <c r="O98" t="s">
         <v>695</v>
       </c>
-      <c r="P98" s="4">
+      <c r="P98" s="3">
         <f t="shared" si="24"/>
         <v>0.99534583664838272</v>
       </c>
-      <c r="Q98" s="4">
+      <c r="Q98" s="3">
         <f t="shared" si="22"/>
         <v>0.79768553303227707</v>
       </c>
-      <c r="R98" s="4">
+      <c r="R98" s="3">
         <f t="shared" si="22"/>
         <v>0.56421273709288511</v>
       </c>
-      <c r="S98" s="4">
+      <c r="S98" s="3">
         <f t="shared" si="22"/>
         <v>0.31871945221183412</v>
       </c>
-      <c r="T98" s="4">
+      <c r="T98" s="3">
         <f t="shared" si="25"/>
         <v>7.5298741738196118E-2</v>
       </c>
-      <c r="U98" s="4">
+      <c r="U98" s="3">
         <f t="shared" si="23"/>
         <v>5.8121714228173513E-2</v>
       </c>
-      <c r="V98" s="4">
+      <c r="V98" s="3">
         <f t="shared" si="23"/>
         <v>3.696884056447499E-2</v>
       </c>
-      <c r="W98" s="4">
+      <c r="W98" s="3">
         <f t="shared" si="23"/>
         <v>2.1014554496092207E-2</v>
       </c>
@@ -9975,35 +9990,35 @@
       <c r="O99" t="s">
         <v>704</v>
       </c>
-      <c r="P99" s="4">
+      <c r="P99" s="3">
         <f t="shared" si="24"/>
         <v>0.90219770659311971</v>
       </c>
-      <c r="Q99" s="4">
+      <c r="Q99" s="3">
         <f t="shared" si="22"/>
         <v>0.78971549357900739</v>
       </c>
-      <c r="R99" s="4">
+      <c r="R99" s="3">
         <f t="shared" si="22"/>
         <v>0.53643730442776627</v>
       </c>
-      <c r="S99" s="4">
+      <c r="S99" s="3">
         <f t="shared" si="22"/>
         <v>0.32410126847632176</v>
       </c>
-      <c r="T99" s="4">
+      <c r="T99" s="3">
         <f t="shared" si="25"/>
         <v>6.3013189039567111E-2</v>
       </c>
-      <c r="U99" s="4">
+      <c r="U99" s="3">
         <f t="shared" si="23"/>
         <v>4.9807730521387657E-2</v>
       </c>
-      <c r="V99" s="4">
+      <c r="V99" s="3">
         <f t="shared" si="23"/>
         <v>3.2773156953473187E-2</v>
       </c>
-      <c r="W99" s="4">
+      <c r="W99" s="3">
         <f t="shared" si="23"/>
         <v>1.7197254728125937E-2</v>
       </c>
@@ -10054,35 +10069,35 @@
       <c r="O100" t="s">
         <v>715</v>
       </c>
-      <c r="P100" s="4">
+      <c r="P100" s="3">
         <f t="shared" si="24"/>
         <v>0.88814976964746617</v>
       </c>
-      <c r="Q100" s="4">
+      <c r="Q100" s="3">
         <f t="shared" si="22"/>
         <v>0.76302768224858941</v>
       </c>
-      <c r="R100" s="4">
+      <c r="R100" s="3">
         <f t="shared" si="22"/>
         <v>0.53055979017775812</v>
       </c>
-      <c r="S100" s="4">
+      <c r="S100" s="3">
         <f t="shared" si="22"/>
         <v>0.33123346270616766</v>
       </c>
-      <c r="T100" s="4">
+      <c r="T100" s="3">
         <f t="shared" si="25"/>
         <v>6.1505676562442185E-2</v>
       </c>
-      <c r="U100" s="4">
+      <c r="U100" s="3">
         <f t="shared" si="23"/>
         <v>4.4414295993058073E-2</v>
       </c>
-      <c r="V100" s="4">
+      <c r="V100" s="3">
         <f t="shared" si="23"/>
         <v>2.9474342993075577E-2</v>
       </c>
-      <c r="W100" s="4">
+      <c r="W100" s="3">
         <f t="shared" si="23"/>
         <v>1.6303794286358208E-2</v>
       </c>
@@ -10133,35 +10148,35 @@
       <c r="O101" t="s">
         <v>724</v>
       </c>
-      <c r="P101" s="4">
+      <c r="P101" s="3">
         <f t="shared" si="24"/>
         <v>0.98424614991542159</v>
       </c>
-      <c r="Q101" s="4">
+      <c r="Q101" s="3">
         <f t="shared" si="22"/>
         <v>0.81236454221877652</v>
       </c>
-      <c r="R101" s="4">
+      <c r="R101" s="3">
         <f t="shared" si="22"/>
         <v>0.55505532844657457</v>
       </c>
-      <c r="S101" s="4">
+      <c r="S101" s="3">
         <f t="shared" si="22"/>
         <v>0.34355176910064844</v>
       </c>
-      <c r="T101" s="4">
+      <c r="T101" s="3">
         <f t="shared" si="25"/>
         <v>6.6954688821539335E-2</v>
       </c>
-      <c r="U101" s="4">
+      <c r="U101" s="3">
         <f t="shared" si="23"/>
         <v>4.7209789963349319E-2</v>
       </c>
-      <c r="V101" s="4">
+      <c r="V101" s="3">
         <f t="shared" si="23"/>
         <v>3.2418461023400062E-2</v>
       </c>
-      <c r="W101" s="4">
+      <c r="W101" s="3">
         <f t="shared" si="23"/>
         <v>1.7475155060614606E-2</v>
       </c>
@@ -10212,35 +10227,35 @@
       <c r="O102" t="s">
         <v>734</v>
       </c>
-      <c r="P102" s="4">
+      <c r="P102" s="3">
         <f t="shared" si="24"/>
         <v>0.90052290052290063</v>
       </c>
-      <c r="Q102" s="4">
+      <c r="Q102" s="3">
         <f t="shared" si="22"/>
         <v>0.79374291601449021</v>
       </c>
-      <c r="R102" s="4">
+      <c r="R102" s="3">
         <f t="shared" si="22"/>
         <v>0.55786617392289028</v>
       </c>
-      <c r="S102" s="4">
+      <c r="S102" s="3">
         <f t="shared" si="22"/>
         <v>0.34834847229321642</v>
       </c>
-      <c r="T102" s="4">
+      <c r="T102" s="3">
         <f t="shared" si="25"/>
         <v>6.1392061392061395E-2</v>
       </c>
-      <c r="U102" s="4">
+      <c r="U102" s="3">
         <f t="shared" si="23"/>
         <v>4.26610703842576E-2</v>
       </c>
-      <c r="V102" s="4">
+      <c r="V102" s="3">
         <f t="shared" si="23"/>
         <v>3.1410299149233843E-2</v>
       </c>
-      <c r="W102" s="4">
+      <c r="W102" s="3">
         <f t="shared" si="23"/>
         <v>1.8364653677111015E-2</v>
       </c>
@@ -10291,35 +10306,35 @@
       <c r="O103" t="s">
         <v>743</v>
       </c>
-      <c r="P103" s="4">
+      <c r="P103" s="3">
         <f t="shared" si="24"/>
         <v>0.97836962223544321</v>
       </c>
-      <c r="Q103" s="4">
+      <c r="Q103" s="3">
         <f t="shared" si="22"/>
         <v>0.80624376596654879</v>
       </c>
-      <c r="R103" s="4">
+      <c r="R103" s="3">
         <f t="shared" si="22"/>
         <v>0.55750266956845917</v>
       </c>
-      <c r="S103" s="4">
+      <c r="S103" s="3">
         <f t="shared" si="22"/>
         <v>0.345882596173197</v>
       </c>
-      <c r="T103" s="4">
+      <c r="T103" s="3">
         <f t="shared" si="25"/>
         <v>6.7233535278443404E-2</v>
       </c>
-      <c r="U103" s="4">
+      <c r="U103" s="3">
         <f t="shared" si="23"/>
         <v>4.735501026587912E-2</v>
       </c>
-      <c r="V103" s="4">
+      <c r="V103" s="3">
         <f t="shared" si="23"/>
         <v>3.2563786465315402E-2</v>
       </c>
-      <c r="W103" s="4">
+      <c r="W103" s="3">
         <f t="shared" si="23"/>
         <v>1.7855041607877511E-2</v>
       </c>
@@ -10328,36 +10343,36 @@
       <c r="A105" t="s">
         <v>220</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D105" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-      <c r="G105" s="2"/>
-      <c r="H105" s="2" t="s">
+      <c r="E105" s="4"/>
+      <c r="F105" s="4"/>
+      <c r="G105" s="4"/>
+      <c r="H105" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I105" s="2"/>
-      <c r="J105" s="2"/>
-      <c r="K105" s="2"/>
-      <c r="L105" s="2" t="s">
+      <c r="I105" s="4"/>
+      <c r="J105" s="4"/>
+      <c r="K105" s="4"/>
+      <c r="L105" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="M105" s="2"/>
-      <c r="N105" s="2"/>
-      <c r="O105" s="2"/>
-      <c r="P105" s="2" t="s">
+      <c r="M105" s="4"/>
+      <c r="N105" s="4"/>
+      <c r="O105" s="4"/>
+      <c r="P105" s="4" t="s">
         <v>856</v>
       </c>
-      <c r="Q105" s="2"/>
-      <c r="R105" s="2"/>
-      <c r="S105" s="2"/>
-      <c r="T105" s="2" t="s">
+      <c r="Q105" s="4"/>
+      <c r="R105" s="4"/>
+      <c r="S105" s="4"/>
+      <c r="T105" s="4" t="s">
         <v>857</v>
       </c>
-      <c r="U105" s="2"/>
-      <c r="V105" s="2"/>
-      <c r="W105" s="2"/>
+      <c r="U105" s="4"/>
+      <c r="V105" s="4"/>
+      <c r="W105" s="4"/>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
@@ -10476,35 +10491,35 @@
       <c r="O107" t="s">
         <v>611</v>
       </c>
-      <c r="P107" s="4">
+      <c r="P107" s="3">
         <f>H107/D107</f>
         <v>0.60442640707354989</v>
       </c>
-      <c r="Q107" s="4">
+      <c r="Q107" s="3">
         <f t="shared" ref="Q107:S120" si="26">I107/E107</f>
         <v>0.33544868071639766</v>
       </c>
-      <c r="R107" s="4">
+      <c r="R107" s="3">
         <f t="shared" si="26"/>
         <v>0.19904008758467656</v>
       </c>
-      <c r="S107" s="4">
+      <c r="S107" s="3">
         <f t="shared" si="26"/>
         <v>0.19018145918581034</v>
       </c>
-      <c r="T107" s="4">
+      <c r="T107" s="3">
         <f>L107/D107</f>
         <v>0.29993360615989811</v>
       </c>
-      <c r="U107" s="4">
+      <c r="U107" s="3">
         <f t="shared" ref="U107:W120" si="27">M107/E107</f>
         <v>0.27741406550645242</v>
       </c>
-      <c r="V107" s="4">
+      <c r="V107" s="3">
         <f t="shared" si="27"/>
         <v>0.24015126231135847</v>
       </c>
-      <c r="W107" s="4">
+      <c r="W107" s="3">
         <f t="shared" si="27"/>
         <v>0.20485708302447489</v>
       </c>
@@ -10555,35 +10570,35 @@
       <c r="O108" t="s">
         <v>621</v>
       </c>
-      <c r="P108" s="4">
+      <c r="P108" s="3">
         <f t="shared" ref="P108:P120" si="28">H108/D108</f>
         <v>0.57928395584320103</v>
       </c>
-      <c r="Q108" s="4">
+      <c r="Q108" s="3">
         <f t="shared" si="26"/>
         <v>0.40940278753577564</v>
       </c>
-      <c r="R108" s="4">
+      <c r="R108" s="3">
         <f t="shared" si="26"/>
         <v>0.23023459897305945</v>
       </c>
-      <c r="S108" s="4">
+      <c r="S108" s="3">
         <f t="shared" si="26"/>
         <v>0.13401010027705323</v>
       </c>
-      <c r="T108" s="4">
+      <c r="T108" s="3">
         <f t="shared" ref="T108:T120" si="29">L108/D108</f>
         <v>0.31673368905325772</v>
       </c>
-      <c r="U108" s="4">
+      <c r="U108" s="3">
         <f t="shared" si="27"/>
         <v>0.2325491544367492</v>
       </c>
-      <c r="V108" s="4">
+      <c r="V108" s="3">
         <f t="shared" si="27"/>
         <v>0.182545708221687</v>
       </c>
-      <c r="W108" s="4">
+      <c r="W108" s="3">
         <f t="shared" si="27"/>
         <v>0.13257716438065723</v>
       </c>
@@ -10634,35 +10649,35 @@
       <c r="O109" t="s">
         <v>633</v>
       </c>
-      <c r="P109" s="4">
+      <c r="P109" s="3">
         <f t="shared" si="28"/>
         <v>0.54722831137579331</v>
       </c>
-      <c r="Q109" s="4">
+      <c r="Q109" s="3">
         <f t="shared" si="26"/>
         <v>0.38474349926205786</v>
       </c>
-      <c r="R109" s="4">
+      <c r="R109" s="3">
         <f t="shared" si="26"/>
         <v>0.22611450261828459</v>
       </c>
-      <c r="S109" s="4">
+      <c r="S109" s="3">
         <f t="shared" si="26"/>
         <v>5.7919098348473724E-2</v>
       </c>
-      <c r="T109" s="4">
+      <c r="T109" s="3">
         <f t="shared" si="29"/>
         <v>0.15928493998133009</v>
       </c>
-      <c r="U109" s="4">
+      <c r="U109" s="3">
         <f t="shared" si="27"/>
         <v>0.12604941696131686</v>
       </c>
-      <c r="V109" s="4">
+      <c r="V109" s="3">
         <f t="shared" si="27"/>
         <v>8.4655889194249143E-2</v>
       </c>
-      <c r="W109" s="4">
+      <c r="W109" s="3">
         <f t="shared" si="27"/>
         <v>7.7097272890239918E-2</v>
       </c>
@@ -10713,35 +10728,35 @@
       <c r="O110" t="s">
         <v>645</v>
       </c>
-      <c r="P110" s="4">
+      <c r="P110" s="3">
         <f t="shared" si="28"/>
         <v>0.70342348083481909</v>
       </c>
-      <c r="Q110" s="4">
+      <c r="Q110" s="3">
         <f t="shared" si="26"/>
         <v>0.46145314221805561</v>
       </c>
-      <c r="R110" s="4">
+      <c r="R110" s="3">
         <f t="shared" si="26"/>
         <v>0.29808382461762051</v>
       </c>
-      <c r="S110" s="4">
+      <c r="S110" s="3">
         <f t="shared" si="26"/>
         <v>0.16426877103626938</v>
       </c>
-      <c r="T110" s="4">
+      <c r="T110" s="3">
         <f t="shared" si="29"/>
         <v>0.16126190942494817</v>
       </c>
-      <c r="U110" s="4">
+      <c r="U110" s="3">
         <f t="shared" si="27"/>
         <v>0.12443771484021644</v>
       </c>
-      <c r="V110" s="4">
+      <c r="V110" s="3">
         <f t="shared" si="27"/>
         <v>0.12265589063378451</v>
       </c>
-      <c r="W110" s="4">
+      <c r="W110" s="3">
         <f t="shared" si="27"/>
         <v>8.3145225186510907E-2</v>
       </c>
@@ -10792,35 +10807,35 @@
       <c r="O111" t="s">
         <v>655</v>
       </c>
-      <c r="P111" s="4">
+      <c r="P111" s="3">
         <f t="shared" si="28"/>
         <v>0.2846584836743028</v>
       </c>
-      <c r="Q111" s="4">
+      <c r="Q111" s="3">
         <f t="shared" si="26"/>
         <v>0.14539211768710503</v>
       </c>
-      <c r="R111" s="4">
+      <c r="R111" s="3">
         <f t="shared" si="26"/>
         <v>8.1543687174209137E-2</v>
       </c>
-      <c r="S111" s="4">
+      <c r="S111" s="3">
         <f t="shared" si="26"/>
         <v>4.4963306604026525E-2</v>
       </c>
-      <c r="T111" s="4">
+      <c r="T111" s="3">
         <f t="shared" si="29"/>
         <v>0.15370009020972475</v>
       </c>
-      <c r="U111" s="4">
+      <c r="U111" s="3">
         <f t="shared" si="27"/>
         <v>9.4860703238805619E-2</v>
       </c>
-      <c r="V111" s="4">
+      <c r="V111" s="3">
         <f t="shared" si="27"/>
         <v>6.4142027586895384E-2</v>
       </c>
-      <c r="W111" s="4">
+      <c r="W111" s="3">
         <f t="shared" si="27"/>
         <v>3.7127621867720666E-2</v>
       </c>
@@ -10871,35 +10886,35 @@
       <c r="O112" t="s">
         <v>666</v>
       </c>
-      <c r="P112" s="4">
+      <c r="P112" s="3">
         <f t="shared" si="28"/>
         <v>0.12444324470238899</v>
       </c>
-      <c r="Q112" s="4">
+      <c r="Q112" s="3">
         <f t="shared" si="26"/>
         <v>7.1002304459807514E-2</v>
       </c>
-      <c r="R112" s="4">
+      <c r="R112" s="3">
         <f t="shared" si="26"/>
         <v>3.4414419627357945E-2</v>
       </c>
-      <c r="S112" s="4">
+      <c r="S112" s="3">
         <f t="shared" si="26"/>
         <v>3.67610404550393E-2</v>
       </c>
-      <c r="T112" s="4">
+      <c r="T112" s="3">
         <f t="shared" si="29"/>
         <v>0.14281147598379129</v>
       </c>
-      <c r="U112" s="4">
+      <c r="U112" s="3">
         <f t="shared" si="27"/>
         <v>8.7247390538159136E-2</v>
       </c>
-      <c r="V112" s="4">
+      <c r="V112" s="3">
         <f t="shared" si="27"/>
         <v>6.8794343603393482E-2</v>
       </c>
-      <c r="W112" s="4">
+      <c r="W112" s="3">
         <f t="shared" si="27"/>
         <v>5.9540893694405544E-2</v>
       </c>
@@ -10950,35 +10965,35 @@
       <c r="O113" t="s">
         <v>676</v>
       </c>
-      <c r="P113" s="4">
+      <c r="P113" s="3">
         <f t="shared" si="28"/>
         <v>0.5625732381288342</v>
       </c>
-      <c r="Q113" s="4">
+      <c r="Q113" s="3">
         <f t="shared" si="26"/>
         <v>0.48292143696629486</v>
       </c>
-      <c r="R113" s="4">
+      <c r="R113" s="3">
         <f t="shared" si="26"/>
         <v>0.40122782472438301</v>
       </c>
-      <c r="S113" s="4">
+      <c r="S113" s="3">
         <f t="shared" si="26"/>
         <v>0.27727291831083256</v>
       </c>
-      <c r="T113" s="4">
+      <c r="T113" s="3">
         <f t="shared" si="29"/>
         <v>0.15567841315022279</v>
       </c>
-      <c r="U113" s="4">
+      <c r="U113" s="3">
         <f t="shared" si="27"/>
         <v>8.2952873686027301E-2</v>
       </c>
-      <c r="V113" s="4">
+      <c r="V113" s="3">
         <f t="shared" si="27"/>
         <v>5.5406570037495106E-2</v>
       </c>
-      <c r="W113" s="4">
+      <c r="W113" s="3">
         <f t="shared" si="27"/>
         <v>3.4689760484914144E-2</v>
       </c>
@@ -11029,35 +11044,35 @@
       <c r="O114" t="s">
         <v>686</v>
       </c>
-      <c r="P114" s="4">
+      <c r="P114" s="3">
         <f t="shared" si="28"/>
         <v>0.60664869683955147</v>
       </c>
-      <c r="Q114" s="4">
+      <c r="Q114" s="3">
         <f t="shared" si="26"/>
         <v>0.4715428964075114</v>
       </c>
-      <c r="R114" s="4">
+      <c r="R114" s="3">
         <f t="shared" si="26"/>
         <v>0.33124701401241297</v>
       </c>
-      <c r="S114" s="4">
+      <c r="S114" s="3">
         <f t="shared" si="26"/>
         <v>0.24145633180358714</v>
       </c>
-      <c r="T114" s="4">
+      <c r="T114" s="3">
         <f t="shared" si="29"/>
         <v>6.8328492893845086E-2</v>
       </c>
-      <c r="U114" s="4">
+      <c r="U114" s="3">
         <f t="shared" si="27"/>
         <v>4.828689010456487E-2</v>
       </c>
-      <c r="V114" s="4">
+      <c r="V114" s="3">
         <f t="shared" si="27"/>
         <v>3.5292870035607729E-2</v>
       </c>
-      <c r="W114" s="4">
+      <c r="W114" s="3">
         <f t="shared" si="27"/>
         <v>2.1995394411668163E-2</v>
       </c>
@@ -11108,35 +11123,35 @@
       <c r="O115" t="s">
         <v>695</v>
       </c>
-      <c r="P115" s="4">
+      <c r="P115" s="3">
         <f t="shared" si="28"/>
         <v>0.68833511899773259</v>
       </c>
-      <c r="Q115" s="4">
+      <c r="Q115" s="3">
         <f t="shared" si="26"/>
         <v>0.5567845308988113</v>
       </c>
-      <c r="R115" s="4">
+      <c r="R115" s="3">
         <f t="shared" si="26"/>
         <v>0.40787329703241176</v>
       </c>
-      <c r="S115" s="4">
+      <c r="S115" s="3">
         <f t="shared" si="26"/>
         <v>0.24693833016080011</v>
       </c>
-      <c r="T115" s="4">
+      <c r="T115" s="3">
         <f t="shared" si="29"/>
         <v>7.7068218420355217E-2</v>
       </c>
-      <c r="U115" s="4">
+      <c r="U115" s="3">
         <f t="shared" si="27"/>
         <v>6.0853395741131217E-2</v>
       </c>
-      <c r="V115" s="4">
+      <c r="V115" s="3">
         <f t="shared" si="27"/>
         <v>4.0443891349033603E-2</v>
       </c>
-      <c r="W115" s="4">
+      <c r="W115" s="3">
         <f t="shared" si="27"/>
         <v>2.4965294940422982E-2</v>
       </c>
@@ -11187,35 +11202,35 @@
       <c r="O116" t="s">
         <v>704</v>
       </c>
-      <c r="P116" s="4">
+      <c r="P116" s="3">
         <f t="shared" si="28"/>
         <v>0.60368786525707541</v>
       </c>
-      <c r="Q116" s="4">
+      <c r="Q116" s="3">
         <f t="shared" si="26"/>
         <v>0.53027383175753029</v>
       </c>
-      <c r="R116" s="4">
+      <c r="R116" s="3">
         <f t="shared" si="26"/>
         <v>0.36866003538807329</v>
       </c>
-      <c r="S116" s="4">
+      <c r="S116" s="3">
         <f t="shared" si="26"/>
         <v>0.24037510996635256</v>
       </c>
-      <c r="T116" s="4">
+      <c r="T116" s="3">
         <f t="shared" si="29"/>
         <v>6.4651528334099415E-2</v>
       </c>
-      <c r="U116" s="4">
+      <c r="U116" s="3">
         <f t="shared" si="27"/>
         <v>5.2173624636738039E-2</v>
       </c>
-      <c r="V116" s="4">
+      <c r="V116" s="3">
         <f t="shared" si="27"/>
         <v>3.5886614700396918E-2</v>
       </c>
-      <c r="W116" s="4">
+      <c r="W116" s="3">
         <f t="shared" si="27"/>
         <v>2.0407422906946766E-2</v>
       </c>
@@ -11266,35 +11281,35 @@
       <c r="O117" t="s">
         <v>715</v>
       </c>
-      <c r="P117" s="4">
+      <c r="P117" s="3">
         <f t="shared" si="28"/>
         <v>0.5589909442395844</v>
       </c>
-      <c r="Q117" s="4">
+      <c r="Q117" s="3">
         <f t="shared" si="26"/>
         <v>0.48299655858816326</v>
       </c>
-      <c r="R117" s="4">
+      <c r="R117" s="3">
         <f t="shared" si="26"/>
         <v>0.34778882903058106</v>
       </c>
-      <c r="S117" s="4">
+      <c r="S117" s="3">
         <f t="shared" si="26"/>
         <v>0.23415979041822232</v>
       </c>
-      <c r="T117" s="4">
+      <c r="T117" s="3">
         <f t="shared" si="29"/>
         <v>6.3227896964382455E-2</v>
       </c>
-      <c r="U117" s="4">
+      <c r="U117" s="3">
         <f t="shared" si="27"/>
         <v>4.6857064667918419E-2</v>
       </c>
-      <c r="V117" s="4">
+      <c r="V117" s="3">
         <f t="shared" si="27"/>
         <v>3.2716532509154891E-2</v>
       </c>
-      <c r="W117" s="4">
+      <c r="W117" s="3">
         <f t="shared" si="27"/>
         <v>1.9670515274160992E-2</v>
       </c>
@@ -11345,35 +11360,35 @@
       <c r="O118" t="s">
         <v>724</v>
       </c>
-      <c r="P118" s="4">
+      <c r="P118" s="3">
         <f t="shared" si="28"/>
         <v>0.60827956591566001</v>
       </c>
-      <c r="Q118" s="4">
+      <c r="Q118" s="3">
         <f t="shared" si="26"/>
         <v>0.50464116354614308</v>
       </c>
-      <c r="R118" s="4">
+      <c r="R118" s="3">
         <f t="shared" si="26"/>
         <v>0.35095153873363993</v>
       </c>
-      <c r="S118" s="4">
+      <c r="S118" s="3">
         <f t="shared" si="26"/>
         <v>0.23065175612030836</v>
       </c>
-      <c r="T118" s="4">
+      <c r="T118" s="3">
         <f t="shared" si="29"/>
         <v>6.8137523549512538E-2</v>
       </c>
-      <c r="U118" s="4">
+      <c r="U118" s="3">
         <f t="shared" si="27"/>
         <v>4.8877877139433305E-2</v>
       </c>
-      <c r="V118" s="4">
+      <c r="V118" s="3">
         <f t="shared" si="27"/>
         <v>3.4709350312463152E-2</v>
       </c>
-      <c r="W118" s="4">
+      <c r="W118" s="3">
         <f t="shared" si="27"/>
         <v>1.9944971587088307E-2</v>
       </c>
@@ -11424,35 +11439,35 @@
       <c r="O119" t="s">
         <v>734</v>
       </c>
-      <c r="P119" s="4">
+      <c r="P119" s="3">
         <f t="shared" si="28"/>
         <v>0.53438019903036493</v>
       </c>
-      <c r="Q119" s="4">
+      <c r="Q119" s="3">
         <f t="shared" si="26"/>
         <v>0.4665486462134375</v>
       </c>
-      <c r="R119" s="4">
+      <c r="R119" s="3">
         <f t="shared" si="26"/>
         <v>0.33285395925244821</v>
       </c>
-      <c r="S119" s="4">
+      <c r="S119" s="3">
         <f t="shared" si="26"/>
         <v>0.22062057907684066</v>
       </c>
-      <c r="T119" s="4">
+      <c r="T119" s="3">
         <f t="shared" si="29"/>
         <v>6.2660882878285279E-2</v>
       </c>
-      <c r="U119" s="4">
+      <c r="U119" s="3">
         <f t="shared" si="27"/>
         <v>4.4132861689444178E-2</v>
       </c>
-      <c r="V119" s="4">
+      <c r="V119" s="3">
         <f t="shared" si="27"/>
         <v>3.3609030048828217E-2</v>
       </c>
-      <c r="W119" s="4">
+      <c r="W119" s="3">
         <f t="shared" si="27"/>
         <v>2.0935706521280149E-2</v>
       </c>
@@ -11503,46 +11518,55 @@
       <c r="O120" t="s">
         <v>743</v>
       </c>
-      <c r="P120" s="4">
+      <c r="P120" s="3">
         <f t="shared" si="28"/>
         <v>0.62386383062403139</v>
       </c>
-      <c r="Q120" s="4">
+      <c r="Q120" s="3">
         <f t="shared" si="26"/>
         <v>0.51572928760553249</v>
       </c>
-      <c r="R120" s="4">
+      <c r="R120" s="3">
         <f t="shared" si="26"/>
         <v>0.3616969742355437</v>
       </c>
-      <c r="S120" s="4">
+      <c r="S120" s="3">
         <f t="shared" si="26"/>
         <v>0.23693585961708791</v>
       </c>
-      <c r="T120" s="4">
+      <c r="T120" s="3">
         <f t="shared" si="29"/>
         <v>6.8309268237089701E-2</v>
       </c>
-      <c r="U120" s="4">
+      <c r="U120" s="3">
         <f t="shared" si="27"/>
         <v>4.8870367154791539E-2</v>
       </c>
-      <c r="V120" s="4">
+      <c r="V120" s="3">
         <f t="shared" si="27"/>
         <v>3.4647863921921492E-2</v>
       </c>
-      <c r="W120" s="4">
+      <c r="W120" s="3">
         <f t="shared" si="27"/>
         <v>2.0140472226839574E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="D105:G105"/>
-    <mergeCell ref="H105:K105"/>
-    <mergeCell ref="L105:O105"/>
-    <mergeCell ref="P105:S105"/>
-    <mergeCell ref="T105:W105"/>
+    <mergeCell ref="T20:W20"/>
+    <mergeCell ref="P37:S37"/>
+    <mergeCell ref="T37:W37"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="D37:G37"/>
+    <mergeCell ref="H37:K37"/>
+    <mergeCell ref="L37:O37"/>
+    <mergeCell ref="P3:S3"/>
+    <mergeCell ref="P20:S20"/>
+    <mergeCell ref="D88:G88"/>
+    <mergeCell ref="H88:K88"/>
+    <mergeCell ref="L88:O88"/>
+    <mergeCell ref="P88:S88"/>
+    <mergeCell ref="T88:W88"/>
     <mergeCell ref="T54:W54"/>
     <mergeCell ref="T71:W71"/>
     <mergeCell ref="L3:O3"/>
@@ -11559,20 +11583,11 @@
     <mergeCell ref="P71:S71"/>
     <mergeCell ref="H20:K20"/>
     <mergeCell ref="L20:O20"/>
-    <mergeCell ref="D88:G88"/>
-    <mergeCell ref="H88:K88"/>
-    <mergeCell ref="L88:O88"/>
-    <mergeCell ref="P88:S88"/>
-    <mergeCell ref="T88:W88"/>
-    <mergeCell ref="T20:W20"/>
-    <mergeCell ref="P37:S37"/>
-    <mergeCell ref="T37:W37"/>
-    <mergeCell ref="T3:W3"/>
-    <mergeCell ref="D37:G37"/>
-    <mergeCell ref="H37:K37"/>
-    <mergeCell ref="L37:O37"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="P20:S20"/>
+    <mergeCell ref="D105:G105"/>
+    <mergeCell ref="H105:K105"/>
+    <mergeCell ref="L105:O105"/>
+    <mergeCell ref="P105:S105"/>
+    <mergeCell ref="T105:W105"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>